<commit_message>
Corrected the call to snyk-protect
</commit_message>
<xml_diff>
--- a/pipeline.xlsx
+++ b/pipeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorich\source\repos\cv-generator\cv-generator-fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5F7D44E-1892-4604-937F-C10FBAD191BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88A9177F-391E-4E23-9568-2190F74E3FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10845" xr2:uid="{85A6193D-6764-4870-9E6C-E861DF98152E}"/>
   </bookViews>
@@ -953,7 +953,7 @@
       <pane xSplit="10" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,17 +2056,20 @@
       </c>
       <c r="K40" t="str">
         <f t="shared" si="4"/>
-        <v>snyk-protect</v>
+        <v>npm-run-all snyk-protect</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">    "prepare": "snyk-protect",</v>
+        <v xml:space="preserve">    "prepare": "npm-run-all snyk-protect",</v>
       </c>
       <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="N40" s="2" t="str">
+        <f>IF(ISBLANK(P40),"",$N$5)</f>
+        <v>npm-run-all</v>
+      </c>
       <c r="O40" s="2" t="str">
         <f t="shared" ref="O40:O71" si="12">IF(ISBLANK(N40),CONCATENATE(" ",$O$3," ")," ")</f>
-        <v xml:space="preserve"> &amp;&amp; </v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="P40" t="s">
         <v>68</v>
@@ -2250,15 +2253,15 @@
         <v>71</v>
       </c>
       <c r="J48" s="1" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E48:I48)</f>
+        <f t="shared" ref="J48:J54" si="13" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E48:I48)</f>
         <v>build-prod-ngsw</v>
       </c>
       <c r="K48" t="str">
-        <f xml:space="preserve"> IF(NOT(COUNTA(P48:V48)),":",_xlfn.TEXTJOIN(O48,TRUE,N48,_xlfn.TEXTJOIN(O48,TRUE,P48:V48)))</f>
+        <f t="shared" ref="K48:K54" si="14" xml:space="preserve"> IF(NOT(COUNTA(P48:V48)),":",_xlfn.TEXTJOIN(O48,TRUE,N48,_xlfn.TEXTJOIN(O48,TRUE,P48:V48)))</f>
         <v>npm-run-all build</v>
       </c>
       <c r="L48" t="str">
-        <f>IF(ISBLANK(J48),"",CONCATENATE("    """,J48,""": ",IF(M48,"""echo ",""""),K48,""","))</f>
+        <f t="shared" ref="L48:L54" si="15">IF(ISBLANK(J48),"",CONCATENATE("    """,J48,""": ",IF(M48,"""echo ",""""),K48,""","))</f>
         <v xml:space="preserve">    "build-prod-ngsw": "npm-run-all build",</v>
       </c>
       <c r="M48" s="2"/>
@@ -2267,7 +2270,7 @@
         <v>npm-run-all</v>
       </c>
       <c r="O48" s="2" t="str">
-        <f>IF(ISBLANK(N48),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O48:O54" si="16">IF(ISBLANK(N48),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P48" t="s">
@@ -2282,15 +2285,15 @@
         <v>72</v>
       </c>
       <c r="J49" s="1" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E49:I49)</f>
+        <f t="shared" si="13"/>
         <v>build-prod-ngsw:staging</v>
       </c>
       <c r="K49" t="str">
-        <f xml:space="preserve"> IF(NOT(COUNTA(P49:V49)),":",_xlfn.TEXTJOIN(O49,TRUE,N49,_xlfn.TEXTJOIN(O49,TRUE,P49:V49)))</f>
+        <f t="shared" si="14"/>
         <v>npm-run-all build:staging</v>
       </c>
       <c r="L49" t="str">
-        <f>IF(ISBLANK(J49),"",CONCATENATE("    """,J49,""": ",IF(M49,"""echo ",""""),K49,""","))</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">    "build-prod-ngsw:staging": "npm-run-all build:staging",</v>
       </c>
       <c r="M49" s="2"/>
@@ -2299,7 +2302,7 @@
         <v>npm-run-all</v>
       </c>
       <c r="O49" s="2" t="str">
-        <f>IF(ISBLANK(N49),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P49" t="s">
@@ -2314,15 +2317,15 @@
         <v>73</v>
       </c>
       <c r="J50" s="1" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E50:I50)</f>
+        <f t="shared" si="13"/>
         <v>postbuild</v>
       </c>
       <c r="K50" t="str">
-        <f xml:space="preserve"> IF(NOT(COUNTA(P50:V50)),":",_xlfn.TEXTJOIN(O50,TRUE,N50,_xlfn.TEXTJOIN(O50,TRUE,P50:V50)))</f>
+        <f t="shared" si="14"/>
         <v>npm-run-all dev:test-phase:integrate:package:action</v>
       </c>
       <c r="L50" t="str">
-        <f>IF(ISBLANK(J50),"",CONCATENATE("    """,J50,""": ",IF(M50,"""echo ",""""),K50,""","))</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">    "postbuild": "npm-run-all dev:test-phase:integrate:package:action",</v>
       </c>
       <c r="M50" s="2"/>
@@ -2331,7 +2334,7 @@
         <v>npm-run-all</v>
       </c>
       <c r="O50" s="2" t="str">
-        <f>IF(ISBLANK(N50),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P50" t="s">
@@ -2346,15 +2349,15 @@
         <v>74</v>
       </c>
       <c r="J51" s="1" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E51:I51)</f>
+        <f t="shared" si="13"/>
         <v>postbuild:staging</v>
       </c>
       <c r="K51" t="str">
-        <f xml:space="preserve"> IF(NOT(COUNTA(P51:V51)),":",_xlfn.TEXTJOIN(O51,TRUE,N51,_xlfn.TEXTJOIN(O51,TRUE,P51:V51)))</f>
+        <f t="shared" si="14"/>
         <v>npm-run-all postbuild</v>
       </c>
       <c r="L51" t="str">
-        <f>IF(ISBLANK(J51),"",CONCATENATE("    """,J51,""": ",IF(M51,"""echo ",""""),K51,""","))</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">    "postbuild:staging": "npm-run-all postbuild",</v>
       </c>
       <c r="M51" s="2"/>
@@ -2363,7 +2366,7 @@
         <v>npm-run-all</v>
       </c>
       <c r="O51" s="2" t="str">
-        <f>IF(ISBLANK(N51),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P51" t="s">
@@ -2378,21 +2381,21 @@
         <v>75</v>
       </c>
       <c r="J52" s="1" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E52:I52)</f>
+        <f t="shared" si="13"/>
         <v>serve-prod-ngsw</v>
       </c>
       <c r="K52" t="str">
-        <f xml:space="preserve"> IF(NOT(COUNTA(P52:V52)),":",_xlfn.TEXTJOIN(O52,TRUE,N52,_xlfn.TEXTJOIN(O52,TRUE,P52:V52)))</f>
+        <f t="shared" si="14"/>
         <v>http-server dist -p 5000</v>
       </c>
       <c r="L52" t="str">
-        <f>IF(ISBLANK(J52),"",CONCATENATE("    """,J52,""": ",IF(M52,"""echo ",""""),K52,""","))</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">    "serve-prod-ngsw": "http-server dist -p 5000",</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2" t="str">
-        <f>IF(ISBLANK(N52),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P52" t="s">
@@ -2407,15 +2410,15 @@
         <v>102</v>
       </c>
       <c r="J53" s="1" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E53:I53)</f>
+        <f t="shared" si="13"/>
         <v>build-n-serve-prod-ngsw</v>
       </c>
       <c r="K53" t="str">
-        <f xml:space="preserve"> IF(NOT(COUNTA(P53:V53)),":",_xlfn.TEXTJOIN(O53,TRUE,N53,_xlfn.TEXTJOIN(O53,TRUE,P53:V53)))</f>
+        <f t="shared" si="14"/>
         <v>npm-run-all build-prod-ngsw serve-prod-ngsw</v>
       </c>
       <c r="L53" t="str">
-        <f>IF(ISBLANK(J53),"",CONCATENATE("    """,J53,""": ",IF(M53,"""echo ",""""),K53,""","))</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">    "build-n-serve-prod-ngsw": "npm-run-all build-prod-ngsw serve-prod-ngsw",</v>
       </c>
       <c r="M53" s="2"/>
@@ -2424,7 +2427,7 @@
         <v>npm-run-all</v>
       </c>
       <c r="O53" s="2" t="str">
-        <f>IF(ISBLANK(N53),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P53" t="s">
@@ -2442,15 +2445,15 @@
         <v>76</v>
       </c>
       <c r="J54" s="1" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E54:I54)</f>
+        <f t="shared" si="13"/>
         <v>postinstall</v>
       </c>
       <c r="K54" t="str">
-        <f xml:space="preserve"> IF(NOT(COUNTA(P54:V54)),":",_xlfn.TEXTJOIN(O54,TRUE,N54,_xlfn.TEXTJOIN(O54,TRUE,P54:V54)))</f>
+        <f t="shared" si="14"/>
         <v>npm-run-all build-prod-ngsw:staging</v>
       </c>
       <c r="L54" t="str">
-        <f>IF(ISBLANK(J54),"",CONCATENATE("    """,J54,""": ",IF(M54,"""echo ",""""),K54,""","))</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">    "postinstall": "npm-run-all build-prod-ngsw:staging",</v>
       </c>
       <c r="M54" s="2"/>
@@ -2459,7 +2462,7 @@
         <v>npm-run-all</v>
       </c>
       <c r="O54" s="2" t="str">
-        <f>IF(ISBLANK(N54),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P54" t="s">
@@ -2708,7 +2711,7 @@
         <v>2</v>
       </c>
       <c r="J64" s="1" t="str">
-        <f t="shared" ref="J64:J75" si="13" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E64:I64)</f>
+        <f t="shared" ref="J64:J75" si="17" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E64:I64)</f>
         <v>test</v>
       </c>
       <c r="K64" t="str">
@@ -2731,7 +2734,7 @@
     </row>
     <row r="65" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J65" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K65" t="str">
@@ -2753,7 +2756,7 @@
         <v>147</v>
       </c>
       <c r="J66" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>ops:deploy:package:dockerize:build:action</v>
       </c>
       <c r="K66" t="str">
@@ -2761,7 +2764,7 @@
         <v>npm-run-all dockerize-build</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" ref="L66:L71" si="14">IF(ISBLANK(J66),"",CONCATENATE("    """,J66,""": ",IF(M66,"""echo ",""""),K66,""","))</f>
+        <f t="shared" ref="L66:L71" si="18">IF(ISBLANK(J66),"",CONCATENATE("    """,J66,""": ",IF(M66,"""echo ",""""),K66,""","))</f>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:build:action": "npm-run-all dockerize-build",</v>
       </c>
       <c r="M66" s="2"/>
@@ -2785,7 +2788,7 @@
         <v>97</v>
       </c>
       <c r="J67" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>dockerize-build</v>
       </c>
       <c r="K67" t="str">
@@ -2793,7 +2796,7 @@
         <v>docker image build -t jorich/cv-generator-fe:%npm_package_version% -t jorich/cv-generator-fe .</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">    "dockerize-build": "docker image build -t jorich/cv-generator-fe:%npm_package_version% -t jorich/cv-generator-fe .",</v>
       </c>
       <c r="M67" s="2"/>
@@ -2814,7 +2817,7 @@
         <v>147</v>
       </c>
       <c r="J68" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>ops:deploy:package:dockerize:push:action</v>
       </c>
       <c r="K68" t="str">
@@ -2822,7 +2825,7 @@
         <v>npm-run-all dockerize-push</v>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:push:action": "npm-run-all dockerize-push",</v>
       </c>
       <c r="M68" s="2"/>
@@ -2846,7 +2849,7 @@
         <v>98</v>
       </c>
       <c r="J69" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>dockerize-push</v>
       </c>
       <c r="K69" t="str">
@@ -2854,7 +2857,7 @@
         <v>docker push jorich/cv-generator-fe:%npm_package_version% &amp;&amp; docker push jorich/cv-generator-fe:latest</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">    "dockerize-push": "docker push jorich/cv-generator-fe:%npm_package_version% &amp;&amp; docker push jorich/cv-generator-fe:latest",</v>
       </c>
       <c r="M69" s="2"/>
@@ -2875,7 +2878,7 @@
         <v>147</v>
       </c>
       <c r="J70" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>ops:deploy:package:provision:action</v>
       </c>
       <c r="K70" t="str">
@@ -2883,7 +2886,7 @@
         <v>npm-run-all provision</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">    "ops:deploy:package:provision:action": "npm-run-all provision",</v>
       </c>
       <c r="M70" s="2"/>
@@ -2907,7 +2910,7 @@
         <v>86</v>
       </c>
       <c r="J71" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>provision</v>
       </c>
       <c r="K71" t="str">
@@ -2915,7 +2918,7 @@
         <v>cd ../cv-generator-life-terraform &amp;&amp; terraform apply</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v xml:space="preserve">    "provision": "cd ../cv-generator-life-terraform &amp;&amp; terraform apply",</v>
       </c>
       <c r="M71" s="2"/>
@@ -2930,7 +2933,7 @@
     </row>
     <row r="72" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J72" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K72" t="str">
@@ -2940,7 +2943,7 @@
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" s="2" t="str">
-        <f t="shared" ref="O72:O103" si="15">IF(ISBLANK(N72),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O72:O75" si="19">IF(ISBLANK(N72),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
     </row>
@@ -2952,7 +2955,7 @@
         <v>100</v>
       </c>
       <c r="J73" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>update:packages</v>
       </c>
       <c r="K73" t="str">
@@ -2960,13 +2963,13 @@
         <v>node wipe-dependencies.js &amp;&amp; rm -rf node_modules &amp;&amp; npm update --save-dev &amp;&amp; npm update --save</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" ref="L73:L128" si="16">IF(ISBLANK(J73),"",CONCATENATE("    """,J73,""": ",IF(M73,"""echo ",""""),K73,""","))</f>
+        <f t="shared" ref="L73:L128" si="20">IF(ISBLANK(J73),"",CONCATENATE("    """,J73,""": ",IF(M73,"""echo ",""""),K73,""","))</f>
         <v xml:space="preserve">    "update:packages": "node wipe-dependencies.js &amp;&amp; rm -rf node_modules &amp;&amp; npm update --save-dev &amp;&amp; npm update --save",</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P73" t="s">
@@ -2975,17 +2978,17 @@
     </row>
     <row r="74" spans="3:16" x14ac:dyDescent="0.25">
       <c r="K74" t="str">
-        <f t="shared" ref="K74:K137" si="17" xml:space="preserve"> IF(NOT(COUNTA(P74:V74)),":",_xlfn.TEXTJOIN(O74,TRUE,N74,_xlfn.TEXTJOIN(O74,TRUE,P74:V74)))</f>
+        <f t="shared" ref="K74:K137" si="21" xml:space="preserve"> IF(NOT(COUNTA(P74:V74)),":",_xlfn.TEXTJOIN(O74,TRUE,N74,_xlfn.TEXTJOIN(O74,TRUE,P74:V74)))</f>
         <v>:</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
     </row>
@@ -2997,21 +3000,21 @@
         <v>147</v>
       </c>
       <c r="J75" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>dev:plan-phase:plan:report:action</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>echo Plan: Include a full SD process in CI/CD pipeline</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:plan-phase:plan:report:action": "echo Plan: Include a full SD process in CI/CD pipeline",</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P75" t="s">
@@ -3026,21 +3029,21 @@
         <v>147</v>
       </c>
       <c r="J76" s="1" t="str">
-        <f t="shared" ref="J76:J82" si="18" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E76:I76)</f>
+        <f t="shared" ref="J76:J82" si="22" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E76:I76)</f>
         <v>dev:plan-phase:update:report:action</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>echo Update: TODO: Update the dependencied to latest</v>
       </c>
       <c r="L76" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:plan-phase:update:report:action": "echo Update: TODO: Update the dependencied to latest",</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2" t="str">
-        <f t="shared" ref="O76:O83" si="19">IF(ISBLANK(N76),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O76:O83" si="23">IF(ISBLANK(N76),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P76" t="s">
@@ -3055,21 +3058,21 @@
         <v>147</v>
       </c>
       <c r="J77" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>dev:code-phase:code:report:action</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>echo TODO: Code: Implement the new features planned</v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:code-phase:code:report:action": "echo TODO: Code: Implement the new features planned",</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P77" t="s">
@@ -3084,21 +3087,21 @@
         <v>147</v>
       </c>
       <c r="J78" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>dev:build-phase:install:report:action</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>echo Install: TODO: Link to install logs</v>
       </c>
       <c r="L78" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:install:report:action": "echo Install: TODO: Link to install logs",</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P78" t="s">
@@ -3113,21 +3116,21 @@
         <v>147</v>
       </c>
       <c r="J79" s="1" t="str">
-        <f t="shared" ref="J79" si="20" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E79:I79)</f>
+        <f t="shared" ref="J79" si="24" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E79:I79)</f>
         <v>dev:build-phase:build:report:action</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>echo Build: TODO: Link to Build logs</v>
       </c>
       <c r="L79" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:build:report:action": "echo Build: TODO: Link to Build logs",</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2" t="str">
-        <f t="shared" ref="O79" si="21">IF(ISBLANK(N79),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O79" si="25">IF(ISBLANK(N79),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P79" t="s">
@@ -3142,21 +3145,21 @@
         <v>147</v>
       </c>
       <c r="J80" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>ops:monitor:report:action</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>echo Observe: TODO: Lanch the observability dashboard</v>
       </c>
       <c r="L80" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "ops:monitor:report:action": "echo Observe: TODO: Lanch the observability dashboard",</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P80" t="s">
@@ -3165,17 +3168,17 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K81" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L81" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2" t="str">
-        <f t="shared" ref="O81" si="22">IF(ISBLANK(N81),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O81" si="26">IF(ISBLANK(N81),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
     </row>
@@ -3187,37 +3190,37 @@
         <v>172</v>
       </c>
       <c r="J82" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>do-nothing</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L82" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "do-nothing": ":",</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K83" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L83" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
     </row>
@@ -3229,21 +3232,21 @@
         <v>101</v>
       </c>
       <c r="J84" s="1" t="str">
-        <f t="shared" ref="J84:J115" si="23" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E84:I84)</f>
+        <f t="shared" ref="J84:J115" si="27" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E84:I84)</f>
         <v>PIPELINE</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:* &amp;&amp; npm-run-all ops:*</v>
       </c>
       <c r="L84" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "PIPELINE": "npm-run-all dev:* &amp;&amp; npm-run-all ops:*",</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2" t="str">
-        <f t="shared" ref="O84:O122" si="24">IF(ISBLANK(N84),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O84:O122" si="28">IF(ISBLANK(N84),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P84" t="s">
@@ -3258,28 +3261,28 @@
         <v>132</v>
       </c>
       <c r="J85" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:*</v>
       </c>
       <c r="L85" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev": "npm-run-all dev:*",</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2" t="str">
-        <f t="shared" ref="N85:N122" si="25">IF(ISBLANK(P85),"",IF(ISNUMBER(SEARCH(":*",P85)),$N$5,$N$3))</f>
+        <f t="shared" ref="N85:N122" si="29">IF(ISBLANK(P85),"",IF(ISNUMBER(SEARCH(":*",P85)),$N$5,$N$3))</f>
         <v>npm-run-all</v>
       </c>
       <c r="O85" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P85" t="str">
-        <f t="shared" ref="P85" si="26">CONCATENATE(IF(CODE(J85)-CODE("a")&lt;0,LOWER(LEFT(J85,IF(ISERR(FIND(":",J85)),LEN(J85)+1,FIND(":",J85))-1)),J85),":*")</f>
+        <f t="shared" ref="P85" si="30">CONCATENATE(IF(CODE(J85)-CODE("a")&lt;0,LOWER(LEFT(J85,IF(ISERR(FIND(":",J85)),LEN(J85)+1,FIND(":",J85))-1)),J85),":*")</f>
         <v>dev:*</v>
       </c>
     </row>
@@ -3300,24 +3303,24 @@
         <v>137</v>
       </c>
       <c r="J86" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:plan-phase</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:plan-phase:*</v>
       </c>
       <c r="L86" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:plan-phase": "npm-run-all dev:plan-phase:*",</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O86" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P86" t="str">
@@ -3336,28 +3339,28 @@
         <v>109</v>
       </c>
       <c r="J87" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:plan-phase:plan</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:plan-phase:plan:*</v>
       </c>
       <c r="L87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:plan-phase:plan": "npm-run-all dev:plan-phase:plan:*",</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O87" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P87" t="str">
-        <f t="shared" ref="P87:P101" si="27">CONCATENATE(IF(CODE(J87)-CODE("a")&lt;0,LOWER(LEFT(J87,IF(ISERR(FIND(":",J87)),LEN(J87)+1,FIND(":",J87))-1)),J87),":*")</f>
+        <f t="shared" ref="P87:P101" si="31">CONCATENATE(IF(CODE(J87)-CODE("a")&lt;0,LOWER(LEFT(J87,IF(ISERR(FIND(":",J87)),LEN(J87)+1,FIND(":",J87))-1)),J87),":*")</f>
         <v>dev:plan-phase:plan:*</v>
       </c>
     </row>
@@ -3375,28 +3378,28 @@
         <v>11</v>
       </c>
       <c r="J88" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:plan-phase:plan:report</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:plan-phase:plan:report:action</v>
       </c>
       <c r="L88" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:plan-phase:plan:report": "npm-run-all dev:plan-phase:plan:report:action",</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O88" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P88" t="str">
-        <f t="shared" ref="P88:P90" si="28" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J88,"action")</f>
+        <f t="shared" ref="P88:P90" si="32" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J88,"action")</f>
         <v>dev:plan-phase:plan:report:action</v>
       </c>
     </row>
@@ -3414,28 +3417,28 @@
         <v>64</v>
       </c>
       <c r="J89" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:plan-phase:update</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:plan-phase:update:*</v>
       </c>
       <c r="L89" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:plan-phase:update": "npm-run-all dev:plan-phase:update:*",</v>
       </c>
       <c r="M89" s="2"/>
       <c r="N89" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O89" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P89" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>dev:plan-phase:update:*</v>
       </c>
     </row>
@@ -3453,28 +3456,28 @@
         <v>11</v>
       </c>
       <c r="J90" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:plan-phase:update:report</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:plan-phase:update:report:action</v>
       </c>
       <c r="L90" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:plan-phase:update:report": "npm-run-all dev:plan-phase:update:report:action",</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O90" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P90" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>dev:plan-phase:update:report:action</v>
       </c>
     </row>
@@ -3495,28 +3498,28 @@
         <v>136</v>
       </c>
       <c r="J91" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:code-phase</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:code-phase:*</v>
       </c>
       <c r="L91" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:code-phase": "npm-run-all dev:code-phase:*",</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O91" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P91" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>dev:code-phase:*</v>
       </c>
     </row>
@@ -3531,28 +3534,28 @@
         <v>110</v>
       </c>
       <c r="J92" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:code-phase:code</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:code-phase:code:*</v>
       </c>
       <c r="L92" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:code-phase:code": "npm-run-all dev:code-phase:code:*",</v>
       </c>
       <c r="M92" s="2"/>
       <c r="N92" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O92" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P92" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>dev:code-phase:code:*</v>
       </c>
     </row>
@@ -3570,28 +3573,28 @@
         <v>11</v>
       </c>
       <c r="J93" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:code-phase:code:report</v>
       </c>
       <c r="K93" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:code-phase:code:report:action</v>
       </c>
       <c r="L93" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:code-phase:code:report": "npm-run-all dev:code-phase:code:report:action",</v>
       </c>
       <c r="M93" s="2"/>
       <c r="N93" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O93" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P93" t="str">
-        <f t="shared" ref="P93" si="29" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J93,"action")</f>
+        <f t="shared" ref="P93" si="33" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J93,"action")</f>
         <v>dev:code-phase:code:report:action</v>
       </c>
     </row>
@@ -3609,28 +3612,28 @@
         <v>135</v>
       </c>
       <c r="J94" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:build-phase:*</v>
       </c>
       <c r="L94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase": "npm-run-all dev:build-phase:*",</v>
       </c>
       <c r="M94" s="2"/>
       <c r="N94" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O94" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P94" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>dev:build-phase:*</v>
       </c>
     </row>
@@ -3648,28 +3651,28 @@
         <v>5</v>
       </c>
       <c r="J95" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:install</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:build-phase:install:*</v>
       </c>
       <c r="L95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:install": "npm-run-all dev:build-phase:install:*",</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O95" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P95" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>dev:build-phase:install:*</v>
       </c>
     </row>
@@ -3687,24 +3690,24 @@
         <v>34</v>
       </c>
       <c r="J96" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:install:prepare</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:install:prepare": ":",</v>
       </c>
       <c r="M96" s="2"/>
       <c r="N96" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O96" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3722,28 +3725,28 @@
         <v>7</v>
       </c>
       <c r="J97" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:install:package</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:build-phase:install:package:*</v>
       </c>
       <c r="L97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:install:package": "npm-run-all dev:build-phase:install:package:*",</v>
       </c>
       <c r="M97" s="2"/>
       <c r="N97" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O97" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P97" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>dev:build-phase:install:package:*</v>
       </c>
     </row>
@@ -3764,24 +3767,24 @@
         <v>6</v>
       </c>
       <c r="J98" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:install:package:environment</v>
       </c>
       <c r="K98" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L98" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:install:package:environment": ":",</v>
       </c>
       <c r="M98" s="2"/>
       <c r="N98" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O98" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3802,24 +3805,24 @@
         <v>7</v>
       </c>
       <c r="J99" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:install:package:package</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L99" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:install:package:package": ":",</v>
       </c>
       <c r="M99" s="2"/>
       <c r="N99" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O99" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3837,28 +3840,28 @@
         <v>11</v>
       </c>
       <c r="J100" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:install:report</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:build-phase:install:report:action</v>
       </c>
       <c r="L100" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:install:report": "npm-run-all dev:build-phase:install:report:action",</v>
       </c>
       <c r="M100" s="2"/>
       <c r="N100" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O100" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P100" t="str">
-        <f t="shared" ref="P100" si="30" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J100,"action")</f>
+        <f t="shared" ref="P100" si="34" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J100,"action")</f>
         <v>dev:build-phase:install:report:action</v>
       </c>
     </row>
@@ -3876,28 +3879,28 @@
         <v>1</v>
       </c>
       <c r="J101" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:build</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:build-phase:build:*</v>
       </c>
       <c r="L101" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:build": "npm-run-all dev:build-phase:build:*",</v>
       </c>
       <c r="M101" s="2"/>
       <c r="N101" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O101" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P101" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>dev:build-phase:build:*</v>
       </c>
     </row>
@@ -3915,24 +3918,24 @@
         <v>7</v>
       </c>
       <c r="J102" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:build:package</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:build-phase:build:package:action</v>
       </c>
       <c r="L102" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:build:package": "npm-run-all dev:build-phase:build:package:action",</v>
       </c>
       <c r="M102" s="2"/>
       <c r="N102" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O102" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P102" t="str">
@@ -3954,28 +3957,28 @@
         <v>11</v>
       </c>
       <c r="J103" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:build-phase:build:report</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:build-phase:build:report:action</v>
       </c>
       <c r="L103" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:build-phase:build:report": "npm-run-all dev:build-phase:build:report:action",</v>
       </c>
       <c r="M103" s="2"/>
       <c r="N103" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O103" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P103" t="str">
-        <f t="shared" ref="P103" si="31" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J103,"action")</f>
+        <f t="shared" ref="P103" si="35" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J103,"action")</f>
         <v>dev:build-phase:build:report:action</v>
       </c>
     </row>
@@ -3996,28 +3999,28 @@
         <v>134</v>
       </c>
       <c r="J104" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:*</v>
       </c>
       <c r="L104" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase": "npm-run-all dev:test-phase:*",</v>
       </c>
       <c r="M104" s="2"/>
       <c r="N104" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O104" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P104" t="str">
-        <f t="shared" ref="P104:P106" si="32">CONCATENATE(IF(CODE(J104)-CODE("a")&lt;0,LOWER(LEFT(J104,IF(ISERR(FIND(":",J104)),LEN(J104)+1,FIND(":",J104))-1)),J104),":*")</f>
+        <f t="shared" ref="P104:P106" si="36">CONCATENATE(IF(CODE(J104)-CODE("a")&lt;0,LOWER(LEFT(J104,IF(ISERR(FIND(":",J104)),LEN(J104)+1,FIND(":",J104))-1)),J104),":*")</f>
         <v>dev:test-phase:*</v>
       </c>
     </row>
@@ -4032,28 +4035,28 @@
         <v>2</v>
       </c>
       <c r="J105" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:test</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:test:*</v>
       </c>
       <c r="L105" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:test": "npm-run-all dev:test-phase:test:*",</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O105" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>dev:test-phase:test:*</v>
       </c>
     </row>
@@ -4071,28 +4074,28 @@
         <v>7</v>
       </c>
       <c r="J106" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:test:package</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:test:package:*</v>
       </c>
       <c r="L106" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:test:package": "npm-run-all dev:test-phase:test:package:*",</v>
       </c>
       <c r="M106" s="2"/>
       <c r="N106" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O106" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P106" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>dev:test-phase:test:package:*</v>
       </c>
     </row>
@@ -4113,28 +4116,28 @@
         <v>8</v>
       </c>
       <c r="J107" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:test:package:vulnerability</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:test:package:vulnerability:action</v>
       </c>
       <c r="L107" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:vulnerability": "npm-run-all dev:test-phase:test:package:vulnerability:action",</v>
       </c>
       <c r="M107" s="2"/>
       <c r="N107" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O107" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P107" t="str">
-        <f t="shared" ref="P107" si="33" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J107,"action")</f>
+        <f t="shared" ref="P107" si="37" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J107,"action")</f>
         <v>dev:test-phase:test:package:vulnerability:action</v>
       </c>
     </row>
@@ -4155,28 +4158,28 @@
         <v>9</v>
       </c>
       <c r="J108" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:test:package:unit</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:test:package:unit:action</v>
       </c>
       <c r="L108" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:unit": "npm-run-all dev:test-phase:test:package:unit:action",</v>
       </c>
       <c r="M108" s="2"/>
       <c r="N108" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O108" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P108" t="str">
-        <f t="shared" ref="P108:P110" si="34" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J108,"action")</f>
+        <f t="shared" ref="P108:P110" si="38" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J108,"action")</f>
         <v>dev:test-phase:test:package:unit:action</v>
       </c>
     </row>
@@ -4197,28 +4200,28 @@
         <v>10</v>
       </c>
       <c r="J109" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:test:package:integration</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:test:package:integration:action</v>
       </c>
       <c r="L109" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:integration": "npm-run-all dev:test-phase:test:package:integration:action",</v>
       </c>
       <c r="M109" s="2"/>
       <c r="N109" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O109" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P109" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>dev:test-phase:test:package:integration:action</v>
       </c>
     </row>
@@ -4236,28 +4239,28 @@
         <v>95</v>
       </c>
       <c r="J110" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:test:measure</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:test:measure:action</v>
       </c>
       <c r="L110" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:test:measure": "npm-run-all dev:test-phase:test:measure:action",</v>
       </c>
       <c r="M110" s="2"/>
       <c r="N110" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O110" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P110" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>dev:test-phase:test:measure:action</v>
       </c>
     </row>
@@ -4275,24 +4278,24 @@
         <v>11</v>
       </c>
       <c r="J111" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:test:report</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L111" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:test:report": ":",</v>
       </c>
       <c r="M111" s="2"/>
       <c r="N111" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O111" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4310,24 +4313,24 @@
         <v>16</v>
       </c>
       <c r="J112" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:codecover</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L112" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:codecover": ":",</v>
       </c>
       <c r="M112" s="2"/>
       <c r="N112" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O112" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4345,28 +4348,28 @@
         <v>7</v>
       </c>
       <c r="J113" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:codecover:package</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:codecover:package:action</v>
       </c>
       <c r="L113" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:codecover:package": "npm-run-all dev:test-phase:codecover:package:action",</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O113" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P113" t="str">
-        <f t="shared" ref="P113" si="35" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J113,"action")</f>
+        <f t="shared" ref="P113" si="39" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J113,"action")</f>
         <v>dev:test-phase:codecover:package:action</v>
       </c>
     </row>
@@ -4384,24 +4387,24 @@
         <v>11</v>
       </c>
       <c r="J114" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:codecover:report</v>
       </c>
       <c r="K114" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L114" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:codecover:report": ":",</v>
       </c>
       <c r="M114" s="2"/>
       <c r="N114" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O114" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4419,28 +4422,28 @@
         <v>3</v>
       </c>
       <c r="J115" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>dev:test-phase:document</v>
       </c>
       <c r="K115" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:document:*</v>
       </c>
       <c r="L115" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:document": "npm-run-all dev:test-phase:document:*",</v>
       </c>
       <c r="M115" s="2"/>
       <c r="N115" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O115" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P115" t="str">
-        <f t="shared" ref="P115" si="36">CONCATENATE(IF(CODE(J115)-CODE("a")&lt;0,LOWER(LEFT(J115,IF(ISERR(FIND(":",J115)),LEN(J115)+1,FIND(":",J115))-1)),J115),":*")</f>
+        <f t="shared" ref="P115" si="40">CONCATENATE(IF(CODE(J115)-CODE("a")&lt;0,LOWER(LEFT(J115,IF(ISERR(FIND(":",J115)),LEN(J115)+1,FIND(":",J115))-1)),J115),":*")</f>
         <v>dev:test-phase:document:*</v>
       </c>
     </row>
@@ -4458,28 +4461,28 @@
         <v>7</v>
       </c>
       <c r="J116" s="1" t="str">
-        <f t="shared" ref="J116:J147" si="37" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E116:I116)</f>
+        <f t="shared" ref="J116:J147" si="41" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E116:I116)</f>
         <v>dev:test-phase:document:package</v>
       </c>
       <c r="K116" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:document:package:action</v>
       </c>
       <c r="L116" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:document:package": "npm-run-all dev:test-phase:document:package:action",</v>
       </c>
       <c r="M116" s="2"/>
       <c r="N116" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O116" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P116" t="str">
-        <f t="shared" ref="P116" si="38" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J116,"action")</f>
+        <f t="shared" ref="P116" si="42" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J116,"action")</f>
         <v>dev:test-phase:document:package:action</v>
       </c>
     </row>
@@ -4497,24 +4500,24 @@
         <v>11</v>
       </c>
       <c r="J117" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>dev:test-phase:document:report</v>
       </c>
       <c r="K117" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L117" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:document:report": ":",</v>
       </c>
       <c r="M117" s="2"/>
       <c r="N117" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O117" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4532,28 +4535,28 @@
         <v>23</v>
       </c>
       <c r="J118" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>dev:test-phase:integrate</v>
       </c>
       <c r="K118" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:integrate:*</v>
       </c>
       <c r="L118" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:integrate": "npm-run-all dev:test-phase:integrate:*",</v>
       </c>
       <c r="M118" s="2"/>
       <c r="N118" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O118" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P118" t="str">
-        <f t="shared" ref="P118" si="39">CONCATENATE(IF(CODE(J118)-CODE("a")&lt;0,LOWER(LEFT(J118,IF(ISERR(FIND(":",J118)),LEN(J118)+1,FIND(":",J118))-1)),J118),":*")</f>
+        <f t="shared" ref="P118" si="43">CONCATENATE(IF(CODE(J118)-CODE("a")&lt;0,LOWER(LEFT(J118,IF(ISERR(FIND(":",J118)),LEN(J118)+1,FIND(":",J118))-1)),J118),":*")</f>
         <v>dev:test-phase:integrate:*</v>
       </c>
     </row>
@@ -4571,28 +4574,28 @@
         <v>7</v>
       </c>
       <c r="J119" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>dev:test-phase:integrate:package</v>
       </c>
       <c r="K119" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all dev:test-phase:integrate:package:action</v>
       </c>
       <c r="L119" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:package": "npm-run-all dev:test-phase:integrate:package:action",</v>
       </c>
       <c r="M119" s="2"/>
       <c r="N119" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>npm-run-all</v>
       </c>
       <c r="O119" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P119" t="str">
-        <f t="shared" ref="P119" si="40" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J119,"action")</f>
+        <f t="shared" ref="P119" si="44" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,J119,"action")</f>
         <v>dev:test-phase:integrate:package:action</v>
       </c>
     </row>
@@ -4610,24 +4613,24 @@
         <v>93</v>
       </c>
       <c r="J120" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>dev:test-phase:integrate:copy</v>
       </c>
       <c r="K120" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L120" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:copy": ":",</v>
       </c>
       <c r="M120" s="2"/>
       <c r="N120" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O120" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4645,24 +4648,24 @@
         <v>2</v>
       </c>
       <c r="J121" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>dev:test-phase:integrate:test</v>
       </c>
       <c r="K121" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L121" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:test": ":",</v>
       </c>
       <c r="M121" s="2"/>
       <c r="N121" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O121" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4680,24 +4683,24 @@
         <v>11</v>
       </c>
       <c r="J122" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>dev:test-phase:integrate:report</v>
       </c>
       <c r="K122" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L122" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:report": ":",</v>
       </c>
       <c r="M122" s="2"/>
       <c r="N122" s="2" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O122" s="2" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4706,24 +4709,24 @@
         <v>131</v>
       </c>
       <c r="J123" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops</v>
       </c>
       <c r="K123" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:*</v>
       </c>
       <c r="L123" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "ops": "npm-run-all ops:*",</v>
       </c>
       <c r="M123" s="2"/>
       <c r="N123" s="2" t="str">
-        <f t="shared" ref="N123:N124" si="41">IF(ISBLANK(P123),"",IF(ISNUMBER(SEARCH(":*",P123)),$N$5,$N$3))</f>
+        <f t="shared" ref="N123:N124" si="45">IF(ISBLANK(P123),"",IF(ISNUMBER(SEARCH(":*",P123)),$N$5,$N$3))</f>
         <v>npm-run-all</v>
       </c>
       <c r="O123" s="2" t="str">
-        <f t="shared" ref="O123" si="42">IF(ISBLANK(N123),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O123" si="46">IF(ISBLANK(N123),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P123" t="str">
@@ -4748,24 +4751,24 @@
         <v>104</v>
       </c>
       <c r="J124" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:release</v>
       </c>
       <c r="K124" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:release:*</v>
       </c>
       <c r="L124" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "ops:release": "npm-run-all ops:release:*",</v>
       </c>
       <c r="M124" s="2"/>
       <c r="N124" s="2" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>npm-run-all</v>
       </c>
       <c r="O124" s="2" t="str">
-        <f t="shared" ref="O124" si="43">IF(ISBLANK(N124),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O124" si="47">IF(ISBLANK(N124),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P124" t="str">
@@ -4784,24 +4787,24 @@
         <v>7</v>
       </c>
       <c r="J125" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:release:package</v>
       </c>
       <c r="K125" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L125" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "ops:release:package": ":",</v>
       </c>
       <c r="M125" s="2"/>
       <c r="N125" s="2" t="str">
-        <f t="shared" ref="N125:N147" si="44">IF(ISBLANK(P125),"",IF(ISNUMBER(SEARCH(":*",P125)),$N$5,$N$3))</f>
+        <f t="shared" ref="N125:N147" si="48">IF(ISBLANK(P125),"",IF(ISNUMBER(SEARCH(":*",P125)),$N$5,$N$3))</f>
         <v/>
       </c>
       <c r="O125" s="2" t="str">
-        <f t="shared" ref="O125:O141" si="45">IF(ISBLANK(N125),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O125:O141" si="49">IF(ISBLANK(N125),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4816,24 +4819,24 @@
         <v>93</v>
       </c>
       <c r="J126" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:release:copy</v>
       </c>
       <c r="K126" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L126" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "ops:release:copy": ":",</v>
       </c>
       <c r="M126" s="2"/>
       <c r="N126" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O126" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4848,24 +4851,24 @@
         <v>11</v>
       </c>
       <c r="J127" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:release:report</v>
       </c>
       <c r="K127" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L127" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "ops:release:report": ":",</v>
       </c>
       <c r="M127" s="2"/>
       <c r="N127" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O127" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4886,28 +4889,28 @@
         <v>4</v>
       </c>
       <c r="J128" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy</v>
       </c>
       <c r="K128" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:deploy:*</v>
       </c>
       <c r="L128" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">    "ops:deploy": "npm-run-all ops:deploy:*",</v>
       </c>
       <c r="M128" s="2"/>
       <c r="N128" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O128" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P128" t="str">
-        <f t="shared" ref="P128:P130" si="46">CONCATENATE(IF(CODE(J128)-CODE("a")&lt;0,LOWER(LEFT(J128,IF(ISERR(FIND(":",J128)),LEN(J128)+1,FIND(":",J128))-1)),J128),":*")</f>
+        <f t="shared" ref="P128:P130" si="50">CONCATENATE(IF(CODE(J128)-CODE("a")&lt;0,LOWER(LEFT(J128,IF(ISERR(FIND(":",J128)),LEN(J128)+1,FIND(":",J128))-1)),J128),":*")</f>
         <v>ops:deploy:*</v>
       </c>
     </row>
@@ -4922,11 +4925,11 @@
         <v>7</v>
       </c>
       <c r="J129" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy:package</v>
       </c>
       <c r="K129" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:deploy:package:*</v>
       </c>
       <c r="L129" t="str">
@@ -4937,15 +4940,15 @@
         <v>1</v>
       </c>
       <c r="N129" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O129" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P129" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>ops:deploy:package:*</v>
       </c>
     </row>
@@ -4963,28 +4966,28 @@
         <v>77</v>
       </c>
       <c r="J130" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy:package:dockerize</v>
       </c>
       <c r="K130" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:deploy:package:dockerize:*</v>
       </c>
       <c r="L130" t="str">
-        <f t="shared" ref="L130:L151" si="47">IF(ISBLANK(J130),"",CONCATENATE("    """,J130,""": ",IF(M130,"""echo ",""""),K130,""","))</f>
+        <f t="shared" ref="L130:L151" si="51">IF(ISBLANK(J130),"",CONCATENATE("    """,J130,""": ",IF(M130,"""echo ",""""),K130,""","))</f>
         <v xml:space="preserve">    "ops:deploy:package:dockerize": "npm-run-all ops:deploy:package:dockerize:*",</v>
       </c>
       <c r="M130" s="2"/>
       <c r="N130" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O130" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P130" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>ops:deploy:package:dockerize:*</v>
       </c>
     </row>
@@ -5005,24 +5008,24 @@
         <v>1</v>
       </c>
       <c r="J131" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy:package:dockerize:build</v>
       </c>
       <c r="K131" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:deploy:package:dockerize:build:action</v>
       </c>
       <c r="L131" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:build": "npm-run-all ops:deploy:package:dockerize:build:action",</v>
       </c>
       <c r="M131" s="2"/>
       <c r="N131" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O131" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P131" t="str">
@@ -5047,24 +5050,24 @@
         <v>87</v>
       </c>
       <c r="J132" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy:package:dockerize:push</v>
       </c>
       <c r="K132" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:deploy:package:dockerize:push:action</v>
       </c>
       <c r="L132" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:push": "npm-run-all ops:deploy:package:dockerize:push:action",</v>
       </c>
       <c r="M132" s="2"/>
       <c r="N132" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O132" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P132" t="str">
@@ -5086,24 +5089,24 @@
         <v>86</v>
       </c>
       <c r="J133" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy:package:provision</v>
       </c>
       <c r="K133" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:deploy:package:provision:action</v>
       </c>
       <c r="L133" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:deploy:package:provision": "npm-run-all ops:deploy:package:provision:action",</v>
       </c>
       <c r="M133" s="2"/>
       <c r="N133" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O133" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P133" t="str">
@@ -5125,24 +5128,24 @@
         <v>116</v>
       </c>
       <c r="J134" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy:package:orchestrate</v>
       </c>
       <c r="K134" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L134" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:deploy:package:orchestrate": ":",</v>
       </c>
       <c r="M134" s="2"/>
       <c r="N134" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O134" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5157,24 +5160,24 @@
         <v>11</v>
       </c>
       <c r="J135" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:deploy:report</v>
       </c>
       <c r="K135" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>:</v>
       </c>
       <c r="L135" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:deploy:report": ":",</v>
       </c>
       <c r="M135" s="2"/>
       <c r="N135" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O135" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5195,28 +5198,28 @@
         <v>12</v>
       </c>
       <c r="J136" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:run</v>
       </c>
       <c r="K136" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:run:*</v>
       </c>
       <c r="L136" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:run": "npm-run-all ops:run:*",</v>
       </c>
       <c r="M136" s="2"/>
       <c r="N136" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O136" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P136" t="str">
-        <f t="shared" ref="P136" si="48">CONCATENATE(IF(CODE(J136)-CODE("a")&lt;0,LOWER(LEFT(J136,IF(ISERR(FIND(":",J136)),LEN(J136)+1,FIND(":",J136))-1)),J136),":*")</f>
+        <f t="shared" ref="P136" si="52">CONCATENATE(IF(CODE(J136)-CODE("a")&lt;0,LOWER(LEFT(J136,IF(ISERR(FIND(":",J136)),LEN(J136)+1,FIND(":",J136))-1)),J136),":*")</f>
         <v>ops:run:*</v>
       </c>
     </row>
@@ -5231,24 +5234,24 @@
         <v>33</v>
       </c>
       <c r="J137" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:run:platform</v>
       </c>
       <c r="K137" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>npm-run-all ops:run:platform:action</v>
       </c>
       <c r="L137" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:run:platform": "npm-run-all ops:run:platform:action",</v>
       </c>
       <c r="M137" s="2"/>
       <c r="N137" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O137" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P137" t="str">
@@ -5267,24 +5270,24 @@
         <v>7</v>
       </c>
       <c r="J138" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:run:package</v>
       </c>
       <c r="K138" t="str">
-        <f t="shared" ref="K138:K150" si="49" xml:space="preserve"> IF(NOT(COUNTA(P138:V138)),":",_xlfn.TEXTJOIN(O138,TRUE,N138,_xlfn.TEXTJOIN(O138,TRUE,P138:V138)))</f>
+        <f t="shared" ref="K138:K150" si="53" xml:space="preserve"> IF(NOT(COUNTA(P138:V138)),":",_xlfn.TEXTJOIN(O138,TRUE,N138,_xlfn.TEXTJOIN(O138,TRUE,P138:V138)))</f>
         <v>:</v>
       </c>
       <c r="L138" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:run:package": ":",</v>
       </c>
       <c r="M138" s="2"/>
       <c r="N138" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O138" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5299,24 +5302,24 @@
         <v>115</v>
       </c>
       <c r="J139" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:run:chaos</v>
       </c>
       <c r="K139" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L139" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:run:chaos": ":",</v>
       </c>
       <c r="M139" s="2"/>
       <c r="N139" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O139" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5331,24 +5334,24 @@
         <v>11</v>
       </c>
       <c r="J140" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:run:report</v>
       </c>
       <c r="K140" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L140" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:run:report": ":",</v>
       </c>
       <c r="M140" s="2"/>
       <c r="N140" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O140" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5369,28 +5372,28 @@
         <v>105</v>
       </c>
       <c r="J141" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:monitor</v>
       </c>
       <c r="K141" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>npm-run-all ops:monitor:*</v>
       </c>
       <c r="L141" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor": "npm-run-all ops:monitor:*",</v>
       </c>
       <c r="M141" s="2"/>
       <c r="N141" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O141" s="2" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P141" t="str">
-        <f t="shared" ref="P141:P144" si="50">CONCATENATE(IF(CODE(J141)-CODE("a")&lt;0,LOWER(LEFT(J141,IF(ISERR(FIND(":",J141)),LEN(J141)+1,FIND(":",J141))-1)),J141),":*")</f>
+        <f t="shared" ref="P141:P144" si="54">CONCATENATE(IF(CODE(J141)-CODE("a")&lt;0,LOWER(LEFT(J141,IF(ISERR(FIND(":",J141)),LEN(J141)+1,FIND(":",J141))-1)),J141),":*")</f>
         <v>ops:monitor:*</v>
       </c>
     </row>
@@ -5405,24 +5408,24 @@
         <v>33</v>
       </c>
       <c r="J142" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:monitor:platform</v>
       </c>
       <c r="K142" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L142" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:platform": ":",</v>
       </c>
       <c r="M142" s="2"/>
       <c r="N142" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O142" s="2" t="str">
-        <f t="shared" ref="O142" si="51">IF(ISBLANK(N142),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O142" si="55">IF(ISBLANK(N142),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5437,28 +5440,28 @@
         <v>7</v>
       </c>
       <c r="J143" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:monitor:package</v>
       </c>
       <c r="K143" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>npm-run-all ops:monitor:package:*</v>
       </c>
       <c r="L143" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:package": "npm-run-all ops:monitor:package:*",</v>
       </c>
       <c r="M143" s="2"/>
       <c r="N143" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O143" s="2" t="str">
-        <f t="shared" ref="O143" si="52">IF(ISBLANK(N143),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O143" si="56">IF(ISBLANK(N143),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P143" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>ops:monitor:package:*</v>
       </c>
     </row>
@@ -5476,28 +5479,28 @@
         <v>117</v>
       </c>
       <c r="J144" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:monitor:package:trail</v>
       </c>
       <c r="K144" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>npm-run-all ops:monitor:package:trail:*</v>
       </c>
       <c r="L144" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:package:trail": "npm-run-all ops:monitor:package:trail:*",</v>
       </c>
       <c r="M144" s="2"/>
       <c r="N144" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>npm-run-all</v>
       </c>
       <c r="O144" s="2" t="str">
-        <f t="shared" ref="O144" si="53">IF(ISBLANK(N144),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O144" si="57">IF(ISBLANK(N144),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P144" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>ops:monitor:package:trail:*</v>
       </c>
     </row>
@@ -5518,24 +5521,24 @@
         <v>111</v>
       </c>
       <c r="J145" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:monitor:package:trail:health</v>
       </c>
       <c r="K145" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L145" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:health": ":",</v>
       </c>
       <c r="M145" s="2"/>
       <c r="N145" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O145" s="2" t="str">
-        <f t="shared" ref="O145" si="54">IF(ISBLANK(N145),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O145" si="58">IF(ISBLANK(N145),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5556,24 +5559,24 @@
         <v>112</v>
       </c>
       <c r="J146" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:monitor:package:trail:performance</v>
       </c>
       <c r="K146" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L146" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:performance": ":",</v>
       </c>
       <c r="M146" s="2"/>
       <c r="N146" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O146" s="2" t="str">
-        <f t="shared" ref="O146" si="55">IF(ISBLANK(N146),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O146" si="59">IF(ISBLANK(N146),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5594,24 +5597,24 @@
         <v>113</v>
       </c>
       <c r="J147" s="1" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>ops:monitor:package:trail:resilience</v>
       </c>
       <c r="K147" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L147" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:resilience": ":",</v>
       </c>
       <c r="M147" s="2"/>
       <c r="N147" s="2" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="O147" s="2" t="str">
-        <f t="shared" ref="O147" si="56">IF(ISBLANK(N147),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O147" si="60">IF(ISBLANK(N147),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5632,24 +5635,24 @@
         <v>114</v>
       </c>
       <c r="J148" s="1" t="str">
-        <f t="shared" ref="J148:J150" si="57" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E148:I148)</f>
+        <f t="shared" ref="J148:J150" si="61" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,E148:I148)</f>
         <v>ops:monitor:package:trail:security</v>
       </c>
       <c r="K148" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L148" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:security": ":",</v>
       </c>
       <c r="M148" s="2"/>
       <c r="N148" s="2" t="str">
-        <f t="shared" ref="N148:N150" si="58">IF(ISBLANK(P148),"",IF(ISNUMBER(SEARCH(":*",P148)),$N$5,$N$3))</f>
+        <f t="shared" ref="N148:N150" si="62">IF(ISBLANK(P148),"",IF(ISNUMBER(SEARCH(":*",P148)),$N$5,$N$3))</f>
         <v/>
       </c>
       <c r="O148" s="2" t="str">
-        <f t="shared" ref="O148" si="59">IF(ISBLANK(N148),CONCATENATE(" ",$O$3," ")," ")</f>
+        <f t="shared" ref="O148" si="63">IF(ISBLANK(N148),CONCATENATE(" ",$O$3," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5667,20 +5670,20 @@
         <v>118</v>
       </c>
       <c r="J149" s="1" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>ops:monitor:package:showcase</v>
       </c>
       <c r="K149" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>:</v>
       </c>
       <c r="L149" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:package:showcase": ":",</v>
       </c>
       <c r="M149" s="2"/>
       <c r="N149" s="2" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="O149" s="2" t="str">
@@ -5699,20 +5702,20 @@
         <v>11</v>
       </c>
       <c r="J150" s="1" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>ops:monitor:report</v>
       </c>
       <c r="K150" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>npm-run-all ops:monitor:report:action</v>
       </c>
       <c r="L150" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve">    "ops:monitor:report": "npm-run-all ops:monitor:report:action",</v>
       </c>
       <c r="M150" s="2"/>
       <c r="N150" s="2" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>npm-run-all</v>
       </c>
       <c r="O150" s="2" t="str">
@@ -5726,7 +5729,7 @@
     </row>
     <row r="151" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L151" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5744,75 +5747,75 @@
         <v>39</v>
       </c>
       <c r="E153">
-        <f>COUNTA(E9:E151)</f>
+        <f t="shared" ref="E153:V153" si="64">COUNTA(E9:E151)</f>
         <v>67</v>
       </c>
       <c r="F153">
-        <f>COUNTA(F9:F151)</f>
+        <f t="shared" si="64"/>
         <v>65</v>
       </c>
       <c r="G153">
-        <f>COUNTA(G9:G151)</f>
+        <f t="shared" si="64"/>
         <v>116</v>
       </c>
       <c r="H153">
-        <f>COUNTA(H9:H151)</f>
+        <f t="shared" si="64"/>
         <v>54</v>
       </c>
       <c r="I153">
-        <f>COUNTA(I9:I151)</f>
+        <f t="shared" si="64"/>
         <v>11</v>
       </c>
       <c r="J153" s="1">
-        <f>COUNTA(J9:J151)</f>
+        <f t="shared" si="64"/>
         <v>130</v>
       </c>
       <c r="K153">
-        <f>COUNTA(K9:K151)</f>
+        <f t="shared" si="64"/>
         <v>142</v>
       </c>
       <c r="L153">
-        <f>COUNTA(L9:L151)</f>
+        <f t="shared" si="64"/>
         <v>141</v>
       </c>
       <c r="M153">
-        <f>COUNTA(M9:M151)</f>
+        <f t="shared" si="64"/>
         <v>2</v>
       </c>
       <c r="N153">
-        <f>COUNTA(N9:N151)</f>
-        <v>89</v>
+        <f t="shared" si="64"/>
+        <v>90</v>
       </c>
       <c r="O153">
-        <f>COUNTA(O9:O151)</f>
+        <f t="shared" si="64"/>
         <v>142</v>
       </c>
       <c r="P153">
-        <f>COUNTA(P9:P151)</f>
+        <f t="shared" si="64"/>
         <v>102</v>
       </c>
       <c r="Q153">
-        <f>COUNTA(Q9:Q151)</f>
+        <f t="shared" si="64"/>
         <v>9</v>
       </c>
       <c r="R153">
-        <f>COUNTA(R9:R151)</f>
+        <f t="shared" si="64"/>
         <v>3</v>
       </c>
       <c r="S153">
-        <f>COUNTA(S9:S151)</f>
+        <f t="shared" si="64"/>
         <v>2</v>
       </c>
       <c r="T153">
-        <f>COUNTA(T9:T151)</f>
+        <f t="shared" si="64"/>
         <v>2</v>
       </c>
       <c r="U153">
-        <f>COUNTA(U9:U151)</f>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="V153">
-        <f>COUNTA(V9:V151)</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Used Chrome headless on some CI
</commit_message>
<xml_diff>
--- a/pipeline.xlsx
+++ b/pipeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorich\AppData\Local\Packages\C27EB4BA.DROPBOX_xbfy0k16fey96\LocalState\users\85455724\FilesCache\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4642E1-C771-4C4E-980B-778AB1D34319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E8E7E7-0691-49F6-A21D-E62C8A5857D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10845" xr2:uid="{85A6193D-6764-4870-9E6C-E861DF98152E}"/>
   </bookViews>
@@ -573,18 +573,12 @@
     <t>git push heroku master</t>
   </si>
   <si>
-    <t>if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then env singleRun=true ng test --code-coverage ; fi</t>
-  </si>
-  <si>
     <t>if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then ng test --code-coverage ; fi</t>
   </si>
   <si>
     <t>if [ ! \"$HEROKU\" ] ; then ng e2e ; fi</t>
   </si>
   <si>
-    <t>if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then cp -r coverage dist/coverage/ ; fi</t>
-  </si>
-  <si>
     <t>if [ ! \"$HEROKU\" ] ; then curl https://cv-generator-fe.herokuapp.com/Webpage ; fi</t>
   </si>
   <si>
@@ -664,6 +658,12 @@
   </si>
   <si>
     <t>if test \"$HEROKU\" ; then npm run heroku-config | grep -v _TOKEN ; fi</t>
+  </si>
+  <si>
+    <t>env singleRun=true ng test --code-coverage</t>
+  </si>
+  <si>
+    <t>cp -r coverage dist/coverage/</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1037,10 @@
   <dimension ref="A1:V170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="K17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="J131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8:K168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1106,7 @@
         <v>101</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>129</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="N3" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
         <v>:</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" ref="K8:K23" si="2">IF(ISBLANK(I8),"",CONCATENATE("    """,I8,""": ",IF(M8,"""echo ",""""),IF(LEN(J8)&gt;1,CONCATENATE(IF(L8,"",N$3)," "),""),J8,""","))</f>
+        <f t="shared" ref="K8" si="2">IF(ISBLANK(I8),"",CONCATENATE("    """,I8,""": ","""",IF(LEN(J8)&gt;1,CONCATENATE(IF(L8,"",CONCATENATE(N$3," ")),""),""),IF(M8,"echo ",""),J8,""","))</f>
         <v xml:space="preserve">    "// TOOLS": ":",</v>
       </c>
       <c r="L8" s="2"/>
@@ -1219,10 +1219,12 @@
         <v>ng</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">    "ng": "date &amp;&amp; time ng",</v>
-      </c>
-      <c r="L9" s="2"/>
+        <f>IF(ISBLANK(I9),"",CONCATENATE("    """,I9,""": ","""",IF(LEN(J9)&gt;1,CONCATENATE(IF(L9,"",CONCATENATE(N$3," ")),""),""),IF(M9,"echo ",""),J9,""","))</f>
+        <v xml:space="preserve">    "ng": "ng",</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="str">
@@ -1246,7 +1248,7 @@
         <v>ng version &amp;&amp; echo Node, NPM and NVM version: &amp;&amp; node -v &amp;&amp; npm -v &amp;&amp; nvm v</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K10:K73" si="3">IF(ISBLANK(I10),"",CONCATENATE("    """,I10,""": ","""",IF(LEN(J10)&gt;1,CONCATENATE(IF(L10,"",CONCATENATE(N$3," ")),""),""),IF(M10,"echo ",""),J10,""","))</f>
         <v xml:space="preserve">    "ver": "date &amp;&amp; time ng version &amp;&amp; echo Node, NPM and NVM version: &amp;&amp; node -v &amp;&amp; npm -v &amp;&amp; nvm v",</v>
       </c>
       <c r="L10" s="2"/>
@@ -1274,7 +1276,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1285,7 +1287,7 @@
         <v>heroku config</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "heroku-config": "date &amp;&amp; time heroku config",</v>
       </c>
       <c r="L11" s="2"/>
@@ -1296,7 +1298,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1307,21 +1309,23 @@
         <v>174</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f t="shared" ref="I12:I18" si="3" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D12:H12)</f>
+        <f t="shared" ref="I12:I18" si="4" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D12:H12)</f>
         <v>build:plain</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12:J18" si="4" xml:space="preserve"> IF(NOT(COUNTA(P12:V12)),":",_xlfn.TEXTJOIN(O12,TRUE,N12,_xlfn.TEXTJOIN(O12,TRUE,P12:V12)))</f>
+        <f t="shared" ref="J12:J18" si="5" xml:space="preserve"> IF(NOT(COUNTA(P12:V12)),":",_xlfn.TEXTJOIN(O12,TRUE,N12,_xlfn.TEXTJOIN(O12,TRUE,P12:V12)))</f>
         <v>npm-run-all build</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">    "build:plain": "date &amp;&amp; time npm-run-all build",</v>
-      </c>
-      <c r="L12" s="2"/>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "build:plain": "npm-run-all build",</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2" t="str">
-        <f t="shared" ref="N12:N18" si="5">IF(ISBLANK(P12),"",$N$6)</f>
+        <f t="shared" ref="N12:N18" si="6">IF(ISBLANK(P12),"",$N$6)</f>
         <v>npm-run-all</v>
       </c>
       <c r="O12" s="2" t="str">
@@ -1340,21 +1344,21 @@
         <v>170</v>
       </c>
       <c r="I13" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>build:full</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="5"/>
+        <v>npm-run-all dev:build-phase</v>
+      </c>
+      <c r="K13" t="str">
         <f t="shared" si="3"/>
-        <v>build:full</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="4"/>
-        <v>npm-run-all dev:build-phase</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="2"/>
         <v xml:space="preserve">    "build:full": "date &amp;&amp; time npm-run-all dev:build-phase",</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>npm-run-all</v>
       </c>
       <c r="O13" s="2" t="str">
@@ -1377,17 +1381,19 @@
         <v>npm run</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>npm-run-all test</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">    "npm run": "date &amp;&amp; time npm-run-all test",</v>
-      </c>
-      <c r="L14" s="2"/>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "npm run": "npm-run-all test",</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>npm-run-all</v>
       </c>
       <c r="O14" s="2" t="str">
@@ -1406,21 +1412,21 @@
         <v>170</v>
       </c>
       <c r="I15" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>test:full</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="5"/>
+        <v>npm-run-all dev:test-phase</v>
+      </c>
+      <c r="K15" t="str">
         <f t="shared" si="3"/>
-        <v>test:full</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="4"/>
-        <v>npm-run-all dev:test-phase</v>
-      </c>
-      <c r="K15" t="str">
-        <f t="shared" si="2"/>
         <v xml:space="preserve">    "test:full": "date &amp;&amp; time npm-run-all dev:test-phase",</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>npm-run-all</v>
       </c>
       <c r="O15" s="2" t="str">
@@ -1439,21 +1445,23 @@
         <v>174</v>
       </c>
       <c r="I16" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>start:plain</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="5"/>
+        <v>npm-run-all start</v>
+      </c>
+      <c r="K16" t="str">
         <f t="shared" si="3"/>
-        <v>start:plain</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="4"/>
-        <v>npm-run-all start</v>
-      </c>
-      <c r="K16" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">    "start:plain": "date &amp;&amp; time npm-run-all start",</v>
-      </c>
-      <c r="L16" s="2"/>
+        <v xml:space="preserve">    "start:plain": "npm-run-all start",</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>npm-run-all</v>
       </c>
       <c r="O16" s="2" t="str">
@@ -1472,21 +1480,21 @@
         <v>170</v>
       </c>
       <c r="I17" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>start:full</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="5"/>
+        <v>npm-run-all ops:run</v>
+      </c>
+      <c r="K17" t="str">
         <f t="shared" si="3"/>
-        <v>start:full</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="4"/>
-        <v>npm-run-all ops:run</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="2"/>
         <v xml:space="preserve">    "start:full": "date &amp;&amp; time npm-run-all ops:run",</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>npm-run-all</v>
       </c>
       <c r="O17" s="2" t="str">
@@ -1502,21 +1510,21 @@
         <v>130</v>
       </c>
       <c r="I18" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>START-PIPELINE</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="5"/>
+        <v>npm-run-all PIPELINE</v>
+      </c>
+      <c r="K18" t="str">
         <f t="shared" si="3"/>
-        <v>START-PIPELINE</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="4"/>
-        <v>npm-run-all PIPELINE</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="2"/>
         <v xml:space="preserve">    "START-PIPELINE": "date &amp;&amp; time npm-run-all PIPELINE",</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>npm-run-all</v>
       </c>
       <c r="O18" s="2" t="str">
@@ -1529,7 +1537,7 @@
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I19" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D19:H19)</f>
@@ -1540,8 +1548,8 @@
         <v>echo CI/CD pipeline START</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">    "pipeline:start:action": " echo CI/CD pipeline START",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "pipeline:start:action": "echo CI/CD pipeline START",</v>
       </c>
       <c r="L19" s="2">
         <v>1</v>
@@ -1553,12 +1561,12 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I20" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D20:H20)</f>
@@ -1569,8 +1577,8 @@
         <v>echo CI/CD pipeline FINISH</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">    "pipeline:finish:action": " echo CI/CD pipeline FINISH",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "pipeline:finish:action": "echo CI/CD pipeline FINISH",</v>
       </c>
       <c r="L20" s="2">
         <v>1</v>
@@ -1582,7 +1590,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
@@ -1591,7 +1599,7 @@
         <v>:</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L21" s="2"/>
@@ -1611,15 +1619,15 @@
         <v>// PLAN</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" ref="I22" si="6" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D22:H22)</f>
+        <f t="shared" ref="I22" si="7" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D22:H22)</f>
         <v>// PLAN</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ref="J22" si="7" xml:space="preserve"> IF(NOT(COUNTA(P22:V22)),":",_xlfn.TEXTJOIN(O22,TRUE,N22,_xlfn.TEXTJOIN(O22,TRUE,P22:V22)))</f>
+        <f t="shared" ref="J22" si="8" xml:space="preserve"> IF(NOT(COUNTA(P22:V22)),":",_xlfn.TEXTJOIN(O22,TRUE,N22,_xlfn.TEXTJOIN(O22,TRUE,P22:V22)))</f>
         <v>:</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "// PLAN": ":",</v>
       </c>
       <c r="L22" s="2"/>
@@ -1643,7 +1651,7 @@
         <v>npm-run-all sys-info:* report-goal</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:plan-phase:plan:report:action": "date &amp;&amp; time npm-run-all sys-info:* report-goal",</v>
       </c>
       <c r="L23" s="2"/>
@@ -1657,18 +1665,18 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="P23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Q23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I24" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D24:H24)</f>
@@ -1679,8 +1687,8 @@
         <v>if test \"$HEROKU\" ; then npm run heroku-config | grep -v _TOKEN ; fi &amp;&amp; if [ \"$HEROKU\" ] ; then env | grep -F HEROKU | grep -Fv _TOKEN ; fi</v>
       </c>
       <c r="K24" t="str">
-        <f>IF(ISBLANK(I24),"",CONCATENATE("    """,I24,""": ",IF(M24,"""echo ",""""),IF(LEN(J24)&gt;1,CONCATENATE(IF(L24,"",N$3)," "),""),J24,""","))</f>
-        <v xml:space="preserve">    "sys-info:heroku": " if test \"$HEROKU\" ; then npm run heroku-config | grep -v _TOKEN ; fi &amp;&amp; if [ \"$HEROKU\" ] ; then env | grep -F HEROKU | grep -Fv _TOKEN ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "sys-info:heroku": "if test \"$HEROKU\" ; then npm run heroku-config | grep -v _TOKEN ; fi &amp;&amp; if [ \"$HEROKU\" ] ; then env | grep -F HEROKU | grep -Fv _TOKEN ; fi",</v>
       </c>
       <c r="L24" s="2">
         <v>1</v>
@@ -1692,7 +1700,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Q24" t="str">
         <f xml:space="preserve"> CONCATENATE("if [ \""$",UPPER($G24),"\"" ] ; then env | grep -F ",UPPER($G24)," | grep -Fv _TOKEN ; fi", "")</f>
@@ -1701,10 +1709,10 @@
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I25" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D25:H25)</f>
@@ -1715,8 +1723,8 @@
         <v>if [ \"$APPVEYOR\" ] ; then env | grep -F APPVEYOR | grep -Fv _TOKEN ; fi</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" ref="K25:K88" si="8">IF(ISBLANK(I25),"",CONCATENATE("    """,I25,""": ",IF(M25,"""echo ",""""),IF(LEN(J25)&gt;1,CONCATENATE(IF(L25,"",N$3)," "),""),J25,""","))</f>
-        <v xml:space="preserve">    "sys-info:appveyor": " if [ \"$APPVEYOR\" ] ; then env | grep -F APPVEYOR | grep -Fv _TOKEN ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "sys-info:appveyor": "if [ \"$APPVEYOR\" ] ; then env | grep -F APPVEYOR | grep -Fv _TOKEN ; fi",</v>
       </c>
       <c r="L25" s="2">
         <v>1</v>
@@ -1734,10 +1742,10 @@
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I26" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D26:H26)</f>
@@ -1748,8 +1756,8 @@
         <v>if [ \"$TRAVIS\" ] ; then env | grep -F TRAVIS | grep -Fv _TOKEN ; fi</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "sys-info:travis": " if [ \"$TRAVIS\" ] ; then env | grep -F TRAVIS | grep -Fv _TOKEN ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "sys-info:travis": "if [ \"$TRAVIS\" ] ; then env | grep -F TRAVIS | grep -Fv _TOKEN ; fi",</v>
       </c>
       <c r="L26" s="2">
         <v>1</v>
@@ -1767,10 +1775,10 @@
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I27" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D27:H27)</f>
@@ -1781,8 +1789,8 @@
         <v>if [ \"$ANGULAR\" ] ; then env | grep -F ANGULAR | grep -Fv _TOKEN ; fi</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "sys-info:angular": " if [ \"$ANGULAR\" ] ; then env | grep -F ANGULAR | grep -Fv _TOKEN ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "sys-info:angular": "if [ \"$ANGULAR\" ] ; then env | grep -F ANGULAR | grep -Fv _TOKEN ; fi",</v>
       </c>
       <c r="L27" s="2">
         <v>1</v>
@@ -1800,10 +1808,10 @@
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I28" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D28:H28)</f>
@@ -1814,8 +1822,8 @@
         <v>if [ \"$NODE\" ] ; then env | grep -F NODE | grep -Fv _TOKEN ; fi</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "sys-info:node": " if [ \"$NODE\" ] ; then env | grep -F NODE | grep -Fv _TOKEN ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "sys-info:node": "if [ \"$NODE\" ] ; then env | grep -F NODE | grep -Fv _TOKEN ; fi",</v>
       </c>
       <c r="L28" s="2">
         <v>1</v>
@@ -1833,10 +1841,10 @@
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I29" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D29:H29)</f>
@@ -1847,8 +1855,8 @@
         <v>if [ \"$NPM\" ] ; then env | grep -F NPM | grep -Fv _TOKEN ; fi</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "sys-info:npm": " if [ \"$NPM\" ] ; then env | grep -F NPM | grep -Fv _TOKEN ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "sys-info:npm": "if [ \"$NPM\" ] ; then env | grep -F NPM | grep -Fv _TOKEN ; fi",</v>
       </c>
       <c r="L29" s="2">
         <v>1</v>
@@ -1866,10 +1874,10 @@
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I30" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D30:H30)</f>
@@ -1880,8 +1888,8 @@
         <v>if [ \"$NVM\" ] ; then env | grep -F NVM | grep -Fv _TOKEN ; fi</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "sys-info:nvm": " if [ \"$NVM\" ] ; then env | grep -F NVM | grep -Fv _TOKEN ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "sys-info:nvm": "if [ \"$NVM\" ] ; then env | grep -F NVM | grep -Fv _TOKEN ; fi",</v>
       </c>
       <c r="L30" s="2">
         <v>1</v>
@@ -1899,7 +1907,7 @@
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I31" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D31:H31)</f>
@@ -1910,7 +1918,7 @@
         <v>echo Plan: Include a full SD process in CI/CD pipeline</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "report-goal": "date &amp;&amp; time echo Plan: Include a full SD process in CI/CD pipeline",</v>
       </c>
       <c r="L31" s="2"/>
@@ -1937,7 +1945,7 @@
         <v>echo Update: TODO: Update the dependencies to latest</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:plan-phase:update:report:action": "date &amp;&amp; time echo Update: TODO: Update the dependencies to latest",</v>
       </c>
       <c r="L32" s="2"/>
@@ -1964,7 +1972,7 @@
         <v>node wipe-dependencies.js &amp;&amp; rm -rf node_modules &amp;&amp; npm update --save-dev &amp;&amp; npm update --save</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "update-packages": "date &amp;&amp; time node wipe-dependencies.js &amp;&amp; rm -rf node_modules &amp;&amp; npm update --save-dev &amp;&amp; npm update --save",</v>
       </c>
       <c r="L33" s="2"/>
@@ -1984,7 +1992,7 @@
         <v>:</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L34" s="2"/>
@@ -2012,7 +2020,7 @@
         <v>:</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "// CODE": ":",</v>
       </c>
       <c r="L35" s="2"/>
@@ -2036,7 +2044,7 @@
         <v>echo TODO: Code: Implement the new features planned</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:code-phase:code:report:action": "date &amp;&amp; time echo TODO: Code: Implement the new features planned",</v>
       </c>
       <c r="L36" s="2"/>
@@ -2056,7 +2064,7 @@
         <v>:</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L37" s="2"/>
@@ -2084,7 +2092,7 @@
         <v>:</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "// BUILD": ":",</v>
       </c>
       <c r="L38" s="2"/>
@@ -2108,7 +2116,7 @@
         <v>if test \"$CI\" ; then snyk auth $SNYK_TOKEN ; fi</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:build-phase:install:prepare:action": "date &amp;&amp; time if test \"$CI\" ; then snyk auth $SNYK_TOKEN ; fi",</v>
       </c>
       <c r="L39" s="2"/>
@@ -2135,7 +2143,7 @@
         <v>snyk protect</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "snyk-protect": "date &amp;&amp; time snyk protect",</v>
       </c>
       <c r="L40" s="2"/>
@@ -2165,7 +2173,7 @@
         <v>npm-run-all snyk-protect</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "prepare": "date &amp;&amp; time npm-run-all snyk-protect",</v>
       </c>
       <c r="L41" s="2"/>
@@ -2195,7 +2203,7 @@
         <v>npm install</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:build-phase:install:package:package:action": "date &amp;&amp; time npm install",</v>
       </c>
       <c r="L42" s="2"/>
@@ -2222,7 +2230,7 @@
         <v>echo Install: TODO: Link to install logs</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:build-phase:install:report:action": "date &amp;&amp; time echo Install: TODO: Link to install logs",</v>
       </c>
       <c r="L43" s="2"/>
@@ -2249,7 +2257,7 @@
         <v>if test \"$CI\" ; then npm run build-ci ; else npm run build ; fi</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:build-phase:build:package:action": "date &amp;&amp; time if test \"$CI\" ; then npm run build-ci ; else npm run build ; fi",</v>
       </c>
       <c r="L44" s="2"/>
@@ -2276,7 +2284,7 @@
         <v>if test \"$CI\" ; then npm run PIPELINE ; else ng build ; fi</v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "build": "date &amp;&amp; time if test \"$CI\" ; then npm run PIPELINE ; else ng build ; fi",</v>
       </c>
       <c r="L45" s="2"/>
@@ -2303,7 +2311,7 @@
         <v>ng build --configuration=\"production\"</v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "build-prod": "date &amp;&amp; time ng build --configuration=\"production\"",</v>
       </c>
       <c r="L46" s="2"/>
@@ -2330,7 +2338,7 @@
         <v>ng build --configuration=\"heroku\"</v>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "build-ci": "date &amp;&amp; time ng build --configuration=\"heroku\"",</v>
       </c>
       <c r="L47" s="2"/>
@@ -2357,7 +2365,7 @@
         <v>git commit --allow-empty -m \"empty commit\" &amp;&amp; git push heroku master</v>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "rebuild-heroku": "date &amp;&amp; time git commit --allow-empty -m \"empty commit\" &amp;&amp; git push heroku master",</v>
       </c>
       <c r="L48" s="2"/>
@@ -2390,7 +2398,7 @@
         <v>auto-changelog -p &amp;&amp; git add CHANGELOG.md</v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "version": "date &amp;&amp; time auto-changelog -p &amp;&amp; git add CHANGELOG.md",</v>
       </c>
       <c r="L49" s="2"/>
@@ -2420,7 +2428,7 @@
         <v>echo Build: TODO: Link to Build logs</v>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:build-phase:build:report:action": "date &amp;&amp; time echo Build: TODO: Link to Build logs",</v>
       </c>
       <c r="L50" s="2"/>
@@ -2440,7 +2448,7 @@
         <v>:</v>
       </c>
       <c r="K51" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L51" s="2"/>
@@ -2468,7 +2476,7 @@
         <v>:</v>
       </c>
       <c r="K52" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "// TEST": ":",</v>
       </c>
       <c r="L52" s="2"/>
@@ -2492,7 +2500,7 @@
         <v>npm-run-all vulnerability-check</v>
       </c>
       <c r="K53" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:vulnerability:action": "date &amp;&amp; time npm-run-all vulnerability-check",</v>
       </c>
       <c r="L53" s="2"/>
@@ -2522,7 +2530,7 @@
         <v>snyk test</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "vulnerability-check": "date &amp;&amp; time snyk test",</v>
       </c>
       <c r="L54" s="2"/>
@@ -2549,7 +2557,7 @@
         <v>npm-run-all test-once</v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:unit:action": "date &amp;&amp; time npm-run-all test-once",</v>
       </c>
       <c r="L55" s="2"/>
@@ -2576,11 +2584,11 @@
       </c>
       <c r="J56" t="str">
         <f t="shared" si="24"/>
-        <v>if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then env singleRun=true ng test --code-coverage ; fi</v>
+        <v>env singleRun=true ng test --code-coverage</v>
       </c>
       <c r="K56" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "test-once": "date &amp;&amp; time if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then env singleRun=true ng test --code-coverage ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "test-once": "date &amp;&amp; time env singleRun=true ng test --code-coverage",</v>
       </c>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
@@ -2590,7 +2598,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P56" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="3:17" x14ac:dyDescent="0.25">
@@ -2609,10 +2617,12 @@
         <v>if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then ng test --code-coverage ; fi</v>
       </c>
       <c r="K57" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "test": "date &amp;&amp; time if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then ng test --code-coverage ; fi",</v>
-      </c>
-      <c r="L57" s="2"/>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "test": "if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then ng test --code-coverage ; fi",</v>
+      </c>
+      <c r="L57" s="2">
+        <v>1</v>
+      </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2" t="str">
@@ -2620,7 +2630,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="3:17" x14ac:dyDescent="0.25">
@@ -2636,7 +2646,7 @@
         <v>npm-run-all e2e</v>
       </c>
       <c r="K58" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:integration:action": "date &amp;&amp; time npm-run-all e2e",</v>
       </c>
       <c r="L58" s="2"/>
@@ -2666,7 +2676,7 @@
         <v>if [ ! \"$HEROKU\" ] ; then ng e2e ; fi</v>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "e2e": "date &amp;&amp; time if [ ! \"$HEROKU\" ] ; then ng e2e ; fi",</v>
       </c>
       <c r="L59" s="2"/>
@@ -2677,7 +2687,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="3:17" x14ac:dyDescent="0.25">
@@ -2693,7 +2703,7 @@
         <v>npm-run-all lint</v>
       </c>
       <c r="K60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:test-phase:test:measure:action": "date &amp;&amp; time npm-run-all lint",</v>
       </c>
       <c r="L60" s="2"/>
@@ -2723,7 +2733,7 @@
         <v>ng  lint</v>
       </c>
       <c r="K61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "lint": "date &amp;&amp; time ng  lint",</v>
       </c>
       <c r="L61" s="2"/>
@@ -2750,7 +2760,7 @@
         <v>npm-run-all codecov coveralls</v>
       </c>
       <c r="K62" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:test-phase:codecover:package:action": "date &amp;&amp; time npm-run-all codecov coveralls",</v>
       </c>
       <c r="L62" s="2"/>
@@ -2783,7 +2793,7 @@
         <v>codecov</v>
       </c>
       <c r="K63" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "codecov": "date &amp;&amp; time codecov",</v>
       </c>
       <c r="L63" s="2"/>
@@ -2810,7 +2820,7 @@
         <v>node ./node_modules/coveralls/bin/coveralls.js &lt; ./coverage/lcov.info</v>
       </c>
       <c r="K64" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "coveralls": "date &amp;&amp; time node ./node_modules/coveralls/bin/coveralls.js &lt; ./coverage/lcov.info",</v>
       </c>
       <c r="L64" s="2"/>
@@ -2837,7 +2847,7 @@
         <v>npm-run-all compodoc</v>
       </c>
       <c r="K65" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:test-phase:document:package:action": "date &amp;&amp; time npm-run-all compodoc",</v>
       </c>
       <c r="L65" s="2"/>
@@ -2867,7 +2877,7 @@
         <v>compodoc -p src/tsconfig.app.json --theme vagrant --hideGenerator --disableSourceCode --disablePrivate --disableTemplateTab --customFavicon \"./src/favicon/android-chrome-512x512.png\" -n \"CV Generator Documentation\"</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "compodoc": "date &amp;&amp; time compodoc -p src/tsconfig.app.json --theme vagrant --hideGenerator --disableSourceCode --disablePrivate --disableTemplateTab --customFavicon \"./src/favicon/android-chrome-512x512.png\" -n \"CV Generator Documentation\"",</v>
       </c>
       <c r="L66" s="2"/>
@@ -2894,7 +2904,7 @@
         <v>npm-run-all ngsw-config ngsw-copy favicon-copy google-copy manifest-copy cov-copy doc-copy</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:package:action": "date &amp;&amp; time npm-run-all ngsw-config ngsw-copy favicon-copy google-copy manifest-copy cov-copy doc-copy",</v>
       </c>
       <c r="L67" s="2"/>
@@ -2942,7 +2952,7 @@
         <v>node_modules/.bin/ngsw-config dist src/ngsw-config.json</v>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "ngsw-config": "date &amp;&amp; time node_modules/.bin/ngsw-config dist src/ngsw-config.json",</v>
       </c>
       <c r="L68" s="2"/>
@@ -2969,7 +2979,7 @@
         <v>cp node_modules/@angular/service-worker/ngsw-worker.js dist/</v>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "ngsw-copy": "date &amp;&amp; time cp node_modules/@angular/service-worker/ngsw-worker.js dist/",</v>
       </c>
       <c r="L69" s="2"/>
@@ -2996,7 +3006,7 @@
         <v>cp src/favicon/* dist/favicon/</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "favicon-copy": "date &amp;&amp; time cp src/favicon/* dist/favicon/",</v>
       </c>
       <c r="L70" s="2"/>
@@ -3023,7 +3033,7 @@
         <v>cp src/google/*.* dist/</v>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "google-copy": "date &amp;&amp; time cp src/google/*.* dist/",</v>
       </c>
       <c r="L71" s="2"/>
@@ -3050,7 +3060,7 @@
         <v>cp src/manifest.json dist/</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    "manifest-copy": "date &amp;&amp; time cp src/manifest.json dist/",</v>
       </c>
       <c r="L72" s="2"/>
@@ -3074,11 +3084,11 @@
       </c>
       <c r="J73" t="str">
         <f t="shared" si="24"/>
-        <v>if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then cp -r coverage dist/coverage/ ; fi</v>
+        <v>cp -r coverage dist/coverage/</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">    "cov-copy": "date &amp;&amp; time if [ ! \"$TRAVIS\" ] &amp;&amp; [ ! \"$HEROKU\" ] ; then cp -r coverage dist/coverage/ ; fi",</v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "cov-copy": "date &amp;&amp; time cp -r coverage dist/coverage/",</v>
       </c>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
@@ -3088,7 +3098,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P73" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
@@ -3104,7 +3114,7 @@
         <v>cp -r documentation dist/documentation/</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K74:K137" si="27">IF(ISBLANK(I74),"",CONCATENATE("    """,I74,""": ","""",IF(LEN(J74)&gt;1,CONCATENATE(IF(L74,"",CONCATENATE(N$3," ")),""),""),IF(M74,"echo ",""),J74,""","))</f>
         <v xml:space="preserve">    "doc-copy": "date &amp;&amp; time cp -r documentation dist/documentation/",</v>
       </c>
       <c r="L74" s="2"/>
@@ -3124,7 +3134,7 @@
         <v>:</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="L75" s="2"/>
@@ -3144,15 +3154,15 @@
         <v>// RELEASE</v>
       </c>
       <c r="I76" s="1" t="str">
-        <f t="shared" ref="I76" si="27" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D76:H76)</f>
+        <f t="shared" ref="I76" si="28" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D76:H76)</f>
         <v>// RELEASE</v>
       </c>
       <c r="J76" t="str">
-        <f t="shared" ref="J76" si="28" xml:space="preserve"> IF(NOT(COUNTA(P76:V76)),":",_xlfn.TEXTJOIN(O76,TRUE,N76,_xlfn.TEXTJOIN(O76,TRUE,P76:V76)))</f>
+        <f t="shared" ref="J76" si="29" xml:space="preserve"> IF(NOT(COUNTA(P76:V76)),":",_xlfn.TEXTJOIN(O76,TRUE,N76,_xlfn.TEXTJOIN(O76,TRUE,P76:V76)))</f>
         <v>:</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "// RELEASE": ":",</v>
       </c>
       <c r="L76" s="2"/>
@@ -3169,7 +3179,7 @@
         <v>:</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="L77" s="2"/>
@@ -3189,15 +3199,15 @@
         <v>// CONFIGURE</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f t="shared" ref="I78" si="29" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D78:H78)</f>
+        <f t="shared" ref="I78" si="30" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D78:H78)</f>
         <v>// CONFIGURE</v>
       </c>
       <c r="J78" t="str">
-        <f t="shared" ref="J78" si="30" xml:space="preserve"> IF(NOT(COUNTA(P78:V78)),":",_xlfn.TEXTJOIN(O78,TRUE,N78,_xlfn.TEXTJOIN(O78,TRUE,P78:V78)))</f>
+        <f t="shared" ref="J78" si="31" xml:space="preserve"> IF(NOT(COUNTA(P78:V78)),":",_xlfn.TEXTJOIN(O78,TRUE,N78,_xlfn.TEXTJOIN(O78,TRUE,P78:V78)))</f>
         <v>:</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "// CONFIGURE": ":",</v>
       </c>
       <c r="L78" s="2"/>
@@ -3213,7 +3223,7 @@
         <v>147</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f t="shared" ref="I79:I84" si="31" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D79:H79)</f>
+        <f t="shared" ref="I79:I84" si="32" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D79:H79)</f>
         <v>ops:deploy:package:dockerize:build:action</v>
       </c>
       <c r="J79" t="str">
@@ -3221,7 +3231,7 @@
         <v>npm-run-all dockerize-build</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:build:action": "date &amp;&amp; time npm-run-all dockerize-build",</v>
       </c>
       <c r="L79" s="2"/>
@@ -3243,7 +3253,7 @@
         <v>78</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>dockerize-build</v>
       </c>
       <c r="J80" t="str">
@@ -3251,7 +3261,7 @@
         <v>docker image build -t jorich/cv-generator-fe:%npm_package_version% -t jorich/cv-generator-fe .</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dockerize-build": "date &amp;&amp; time docker image build -t jorich/cv-generator-fe:%npm_package_version% -t jorich/cv-generator-fe .",</v>
       </c>
       <c r="L80" s="2"/>
@@ -3270,7 +3280,7 @@
         <v>148</v>
       </c>
       <c r="I81" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>ops:deploy:package:dockerize:push:action</v>
       </c>
       <c r="J81" t="str">
@@ -3278,7 +3288,7 @@
         <v>npm-run-all dockerize-push</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:push:action": "date &amp;&amp; time npm-run-all dockerize-push",</v>
       </c>
       <c r="L81" s="2"/>
@@ -3300,7 +3310,7 @@
         <v>79</v>
       </c>
       <c r="I82" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>dockerize-push</v>
       </c>
       <c r="J82" t="str">
@@ -3308,7 +3318,7 @@
         <v>docker push jorich/cv-generator-fe:%npm_package_version% &amp;&amp; docker push jorich/cv-generator-fe:latest</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dockerize-push": "date &amp;&amp; time docker push jorich/cv-generator-fe:%npm_package_version% &amp;&amp; docker push jorich/cv-generator-fe:latest",</v>
       </c>
       <c r="L82" s="2"/>
@@ -3327,7 +3337,7 @@
         <v>149</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>ops:deploy:package:provision:action</v>
       </c>
       <c r="J83" t="str">
@@ -3335,7 +3345,7 @@
         <v>npm-run-all provision</v>
       </c>
       <c r="K83" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "ops:deploy:package:provision:action": "date &amp;&amp; time npm-run-all provision",</v>
       </c>
       <c r="L83" s="2"/>
@@ -3357,7 +3367,7 @@
         <v>69</v>
       </c>
       <c r="I84" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>provision</v>
       </c>
       <c r="J84" t="str">
@@ -3365,7 +3375,7 @@
         <v>cd ../cv-generator-life-terraform &amp;&amp; terraform apply</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "provision": "date &amp;&amp; time cd ../cv-generator-life-terraform &amp;&amp; terraform apply",</v>
       </c>
       <c r="L84" s="2"/>
@@ -3385,7 +3395,7 @@
         <v>:</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="L85" s="2"/>
@@ -3405,15 +3415,15 @@
         <v>// OPERATE</v>
       </c>
       <c r="I86" s="1" t="str">
-        <f t="shared" ref="I86" si="32" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D86:H86)</f>
+        <f t="shared" ref="I86" si="33" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D86:H86)</f>
         <v>// OPERATE</v>
       </c>
       <c r="J86" t="str">
-        <f t="shared" ref="J86" si="33" xml:space="preserve"> IF(NOT(COUNTA(P86:V86)),":",_xlfn.TEXTJOIN(O86,TRUE,N86,_xlfn.TEXTJOIN(O86,TRUE,P86:V86)))</f>
+        <f t="shared" ref="J86" si="34" xml:space="preserve"> IF(NOT(COUNTA(P86:V86)),":",_xlfn.TEXTJOIN(O86,TRUE,N86,_xlfn.TEXTJOIN(O86,TRUE,P86:V86)))</f>
         <v>:</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "// OPERATE": ":",</v>
       </c>
       <c r="L86" s="2"/>
@@ -3437,7 +3447,7 @@
         <v>npm-run-all wake-up-the-dynos:*</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "ops:run:platform:action": "date &amp;&amp; time npm-run-all wake-up-the-dynos:*",</v>
       </c>
       <c r="L87" s="2"/>
@@ -3456,10 +3466,10 @@
     </row>
     <row r="88" spans="3:20" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G88" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I88" s="1" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D88:H88)</f>
@@ -3470,7 +3480,7 @@
         <v>if [ ! \"$HEROKU\" ] ; then curl https://cv-generator-fe.herokuapp.com/Webpage ; fi</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "wake-up-the-dynos:heroku": "date &amp;&amp; time if [ ! \"$HEROKU\" ] ; then curl https://cv-generator-fe.herokuapp.com/Webpage ; fi",</v>
       </c>
       <c r="L88" s="2"/>
@@ -3481,26 +3491,26 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P88" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="3:20" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G89" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I89" s="1" t="str">
-        <f t="shared" ref="I89" si="34" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D89:H89)</f>
+        <f t="shared" ref="I89" si="35" xml:space="preserve"> _xlfn.TEXTJOIN(":",TRUE,D89:H89)</f>
         <v>wake-up-the-dynos:ml</v>
       </c>
       <c r="J89" t="str">
-        <f t="shared" ref="J89" si="35" xml:space="preserve"> IF(NOT(COUNTA(P89:V89)),":",_xlfn.TEXTJOIN(O89,TRUE,N89,_xlfn.TEXTJOIN(O89,TRUE,P89:V89)))</f>
+        <f t="shared" ref="J89" si="36" xml:space="preserve"> IF(NOT(COUNTA(P89:V89)),":",_xlfn.TEXTJOIN(O89,TRUE,N89,_xlfn.TEXTJOIN(O89,TRUE,P89:V89)))</f>
         <v>if [ ! \"$CI\" ] ; then curl cvgenerator.ml ; fi</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" ref="K89:K152" si="36">IF(ISBLANK(I89),"",CONCATENATE("    """,I89,""": ",IF(M89,"""echo ",""""),IF(LEN(J89)&gt;1,CONCATENATE(IF(L89,"",N$3)," "),""),J89,""","))</f>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "wake-up-the-dynos:ml": "date &amp;&amp; time if [ ! \"$CI\" ] ; then curl cvgenerator.ml ; fi",</v>
       </c>
       <c r="L89" s="2"/>
@@ -3511,7 +3521,7 @@
         <v xml:space="preserve"> &amp;&amp; </v>
       </c>
       <c r="P89" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="3:20" x14ac:dyDescent="0.25">
@@ -3530,10 +3540,12 @@
         <v>node server.js</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">    "start": "date &amp;&amp; time node server.js",</v>
-      </c>
-      <c r="L90" s="2"/>
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">    "start": "node server.js",</v>
+      </c>
+      <c r="L90" s="2">
+        <v>1</v>
+      </c>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2" t="str">
@@ -3550,7 +3562,7 @@
         <v>:</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="L91" s="2"/>
@@ -3578,7 +3590,7 @@
         <v>:</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "// OBSERVE": ":",</v>
       </c>
       <c r="L92" s="2"/>
@@ -3602,7 +3614,7 @@
         <v>echo Observe: TODO: Lanch the observability dashboard</v>
       </c>
       <c r="K93" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "ops:monitor:report:action": "date &amp;&amp; time echo Observe: TODO: Lanch the observability dashboard",</v>
       </c>
       <c r="L93" s="2"/>
@@ -3622,7 +3634,7 @@
         <v>:</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="L94" s="2"/>
@@ -3649,7 +3661,7 @@
         <v>npm-run-all pipeline:start dev ops report pipeline:finish</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "PIPELINE": "date &amp;&amp; time npm-run-all pipeline:start dev ops report pipeline:finish",</v>
       </c>
       <c r="L95" s="2"/>
@@ -3663,7 +3675,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="P95" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q95" t="s">
         <v>111</v>
@@ -3675,12 +3687,12 @@
         <v>11</v>
       </c>
       <c r="T95" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E96" t="s">
         <v>0</v>
@@ -3694,7 +3706,7 @@
         <v>npm-run-all pipeline:start:action</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "pipeline:start": "date &amp;&amp; time npm-run-all pipeline:start:action",</v>
       </c>
       <c r="L96" s="2"/>
@@ -3725,7 +3737,7 @@
         <v>npm-run-all dev:*</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev": "date &amp;&amp; time npm-run-all dev:*",</v>
       </c>
       <c r="L97" s="2"/>
@@ -3768,7 +3780,7 @@
         <v>npm-run-all dev:plan-phase:*</v>
       </c>
       <c r="K98" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:plan-phase": "date &amp;&amp; time npm-run-all dev:plan-phase:*",</v>
       </c>
       <c r="L98" s="2"/>
@@ -3805,7 +3817,7 @@
         <v>npm-run-all dev:plan-phase:plan:*</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:plan-phase:plan": "date &amp;&amp; time npm-run-all dev:plan-phase:plan:*",</v>
       </c>
       <c r="L99" s="2"/>
@@ -3845,7 +3857,7 @@
         <v>npm-run-all dev:plan-phase:plan:report:action</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:plan-phase:plan:report": "date &amp;&amp; time npm-run-all dev:plan-phase:plan:report:action",</v>
       </c>
       <c r="L100" s="2"/>
@@ -3885,7 +3897,7 @@
         <v>npm-run-all dev:plan-phase:update:*</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:plan-phase:update": "date &amp;&amp; time npm-run-all dev:plan-phase:update:*",</v>
       </c>
       <c r="L101" s="2"/>
@@ -3925,7 +3937,7 @@
         <v>npm-run-all dev:plan-phase:update:report:action</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:plan-phase:update:report": "date &amp;&amp; time npm-run-all dev:plan-phase:update:report:action",</v>
       </c>
       <c r="L102" s="2"/>
@@ -3968,7 +3980,7 @@
         <v>npm-run-all dev:code-phase:*</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:code-phase": "date &amp;&amp; time npm-run-all dev:code-phase:*",</v>
       </c>
       <c r="L103" s="2"/>
@@ -4005,7 +4017,7 @@
         <v>npm-run-all dev:code-phase:code:*</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:code-phase:code": "date &amp;&amp; time npm-run-all dev:code-phase:code:*",</v>
       </c>
       <c r="L104" s="2"/>
@@ -4045,7 +4057,7 @@
         <v>npm-run-all dev:code-phase:code:report:action</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:code-phase:code:report": "date &amp;&amp; time npm-run-all dev:code-phase:code:report:action",</v>
       </c>
       <c r="L105" s="2"/>
@@ -4085,7 +4097,7 @@
         <v>npm-run-all dev:build-phase:*</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase": "date &amp;&amp; time npm-run-all dev:build-phase:*",</v>
       </c>
       <c r="L106" s="2"/>
@@ -4125,7 +4137,7 @@
         <v>npm-run-all dev:build-phase:install:*</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:install": "date &amp;&amp; time npm-run-all dev:build-phase:install:*",</v>
       </c>
       <c r="L107" s="2"/>
@@ -4165,7 +4177,7 @@
         <v>npm-run-all dev:build-phase:install:prepare:action</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:install:prepare": "date &amp;&amp; time npm-run-all dev:build-phase:install:prepare:action",</v>
       </c>
       <c r="L108" s="2"/>
@@ -4205,7 +4217,7 @@
         <v>npm-run-all dev:build-phase:install:package:*</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:install:package": "date &amp;&amp; time npm-run-all dev:build-phase:install:package:*",</v>
       </c>
       <c r="L109" s="2"/>
@@ -4248,7 +4260,7 @@
         <v>:</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:install:package:environment": ":",</v>
       </c>
       <c r="L110" s="2"/>
@@ -4287,7 +4299,7 @@
         <v>npm-run-all dev:build-phase:install:package:package:action</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:install:package:package": "date &amp;&amp; time npm-run-all dev:build-phase:install:package:package:action",</v>
       </c>
       <c r="L111" s="2"/>
@@ -4327,7 +4339,7 @@
         <v>npm-run-all dev:build-phase:install:report:action</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:install:report": "date &amp;&amp; time npm-run-all dev:build-phase:install:report:action",</v>
       </c>
       <c r="L112" s="2"/>
@@ -4367,7 +4379,7 @@
         <v>npm-run-all dev:build-phase:build:*</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:build": "date &amp;&amp; time npm-run-all dev:build-phase:build:*",</v>
       </c>
       <c r="L113" s="2"/>
@@ -4407,7 +4419,7 @@
         <v>npm-run-all dev:build-phase:build:package:action</v>
       </c>
       <c r="K114" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:build:package": "date &amp;&amp; time npm-run-all dev:build-phase:build:package:action",</v>
       </c>
       <c r="L114" s="2"/>
@@ -4447,7 +4459,7 @@
         <v>npm-run-all dev:build-phase:build:report:action</v>
       </c>
       <c r="K115" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:build-phase:build:report": "date &amp;&amp; time npm-run-all dev:build-phase:build:report:action",</v>
       </c>
       <c r="L115" s="2"/>
@@ -4490,7 +4502,7 @@
         <v>npm-run-all dev:test-phase:*</v>
       </c>
       <c r="K116" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase": "date &amp;&amp; time npm-run-all dev:test-phase:*",</v>
       </c>
       <c r="L116" s="2"/>
@@ -4527,7 +4539,7 @@
         <v>npm-run-all dev:test-phase:test:*</v>
       </c>
       <c r="K117" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:test": "date &amp;&amp; time npm-run-all dev:test-phase:test:*",</v>
       </c>
       <c r="L117" s="2"/>
@@ -4567,7 +4579,7 @@
         <v>npm-run-all dev:test-phase:test:package:*</v>
       </c>
       <c r="K118" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:test:package": "date &amp;&amp; time npm-run-all dev:test-phase:test:package:*",</v>
       </c>
       <c r="L118" s="2"/>
@@ -4610,7 +4622,7 @@
         <v>npm-run-all dev:test-phase:test:package:vulnerability:action</v>
       </c>
       <c r="K119" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:vulnerability": "date &amp;&amp; time npm-run-all dev:test-phase:test:package:vulnerability:action",</v>
       </c>
       <c r="L119" s="2"/>
@@ -4653,7 +4665,7 @@
         <v>npm-run-all dev:test-phase:test:package:unit:action</v>
       </c>
       <c r="K120" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:unit": "date &amp;&amp; time npm-run-all dev:test-phase:test:package:unit:action",</v>
       </c>
       <c r="L120" s="2"/>
@@ -4696,7 +4708,7 @@
         <v>npm-run-all dev:test-phase:test:package:integration:action</v>
       </c>
       <c r="K121" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:test:package:integration": "date &amp;&amp; time npm-run-all dev:test-phase:test:package:integration:action",</v>
       </c>
       <c r="L121" s="2"/>
@@ -4736,7 +4748,7 @@
         <v>npm-run-all dev:test-phase:test:measure:action</v>
       </c>
       <c r="K122" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:test:measure": "date &amp;&amp; time npm-run-all dev:test-phase:test:measure:action",</v>
       </c>
       <c r="L122" s="2"/>
@@ -4776,7 +4788,7 @@
         <v>:</v>
       </c>
       <c r="K123" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:test:report": ":",</v>
       </c>
       <c r="L123" s="2"/>
@@ -4812,7 +4824,7 @@
         <v>:</v>
       </c>
       <c r="K124" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:codecover": ":",</v>
       </c>
       <c r="L124" s="2"/>
@@ -4848,7 +4860,7 @@
         <v>npm-run-all dev:test-phase:codecover:package:action</v>
       </c>
       <c r="K125" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:codecover:package": "date &amp;&amp; time npm-run-all dev:test-phase:codecover:package:action",</v>
       </c>
       <c r="L125" s="2"/>
@@ -4888,7 +4900,7 @@
         <v>:</v>
       </c>
       <c r="K126" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:codecover:report": ":",</v>
       </c>
       <c r="L126" s="2"/>
@@ -4924,7 +4936,7 @@
         <v>npm-run-all dev:test-phase:document:*</v>
       </c>
       <c r="K127" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:document": "date &amp;&amp; time npm-run-all dev:test-phase:document:*",</v>
       </c>
       <c r="L127" s="2"/>
@@ -4964,7 +4976,7 @@
         <v>npm-run-all dev:test-phase:document:package:action</v>
       </c>
       <c r="K128" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:document:package": "date &amp;&amp; time npm-run-all dev:test-phase:document:package:action",</v>
       </c>
       <c r="L128" s="2"/>
@@ -5004,7 +5016,7 @@
         <v>:</v>
       </c>
       <c r="K129" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:document:report": ":",</v>
       </c>
       <c r="L129" s="2"/>
@@ -5040,7 +5052,7 @@
         <v>npm-run-all dev:test-phase:integrate:*</v>
       </c>
       <c r="K130" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:integrate": "date &amp;&amp; time npm-run-all dev:test-phase:integrate:*",</v>
       </c>
       <c r="L130" s="2"/>
@@ -5080,7 +5092,7 @@
         <v>npm-run-all dev:test-phase:integrate:package:action</v>
       </c>
       <c r="K131" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:package": "date &amp;&amp; time npm-run-all dev:test-phase:integrate:package:action",</v>
       </c>
       <c r="L131" s="2"/>
@@ -5120,7 +5132,7 @@
         <v>:</v>
       </c>
       <c r="K132" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:copy": ":",</v>
       </c>
       <c r="L132" s="2"/>
@@ -5156,7 +5168,7 @@
         <v>:</v>
       </c>
       <c r="K133" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:test": ":",</v>
       </c>
       <c r="L133" s="2"/>
@@ -5192,7 +5204,7 @@
         <v>:</v>
       </c>
       <c r="K134" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:integrate:report": ":",</v>
       </c>
       <c r="L134" s="2"/>
@@ -5225,7 +5237,7 @@
         <v>:</v>
       </c>
       <c r="K135" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:test-phase:report": ":",</v>
       </c>
       <c r="L135" s="2"/>
@@ -5255,7 +5267,7 @@
         <v>:</v>
       </c>
       <c r="K136" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "dev:report": ":",</v>
       </c>
       <c r="L136" s="2"/>
@@ -5282,7 +5294,7 @@
         <v>npm-run-all ops:*</v>
       </c>
       <c r="K137" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">    "ops": "date &amp;&amp; time npm-run-all ops:*",</v>
       </c>
       <c r="L137" s="2"/>
@@ -5325,7 +5337,7 @@
         <v>npm-run-all ops:release:*</v>
       </c>
       <c r="K138" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="K138:K168" si="73">IF(ISBLANK(I138),"",CONCATENATE("    """,I138,""": ","""",IF(LEN(J138)&gt;1,CONCATENATE(IF(L138,"",CONCATENATE(N$3," ")),""),""),IF(M138,"echo ",""),J138,""","))</f>
         <v xml:space="preserve">    "ops:release": "date &amp;&amp; time npm-run-all ops:release:*",</v>
       </c>
       <c r="L138" s="2"/>
@@ -5335,7 +5347,7 @@
         <v>npm-run-all</v>
       </c>
       <c r="O138" s="2" t="str">
-        <f t="shared" ref="O138" si="73">IF(ISBLANK(N138),CONCATENATE(" ",$O$4," ")," ")</f>
+        <f t="shared" ref="O138" si="74">IF(ISBLANK(N138),CONCATENATE(" ",$O$4," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P138" t="str">
@@ -5362,17 +5374,17 @@
         <v>:</v>
       </c>
       <c r="K139" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:release:package": ":",</v>
       </c>
       <c r="L139" s="2"/>
       <c r="M139" s="2"/>
       <c r="N139" s="2" t="str">
-        <f t="shared" ref="N139:N161" si="74">IF(ISBLANK(P139),"",IF(ISNUMBER(SEARCH(":*",P139)),$N$6,$N$4))</f>
+        <f t="shared" ref="N139:N161" si="75">IF(ISBLANK(P139),"",IF(ISNUMBER(SEARCH(":*",P139)),$N$6,$N$4))</f>
         <v/>
       </c>
       <c r="O139" s="2" t="str">
-        <f t="shared" ref="O139:O155" si="75">IF(ISBLANK(N139),CONCATENATE(" ",$O$4," ")," ")</f>
+        <f t="shared" ref="O139:O155" si="76">IF(ISBLANK(N139),CONCATENATE(" ",$O$4," ")," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5395,17 +5407,17 @@
         <v>:</v>
       </c>
       <c r="K140" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:release:copy": ":",</v>
       </c>
       <c r="L140" s="2"/>
       <c r="M140" s="2"/>
       <c r="N140" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O140" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5428,17 +5440,17 @@
         <v>:</v>
       </c>
       <c r="K141" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:release:report": ":",</v>
       </c>
       <c r="L141" s="2"/>
       <c r="M141" s="2"/>
       <c r="N141" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O141" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5467,21 +5479,21 @@
         <v>npm-run-all ops:deploy:*</v>
       </c>
       <c r="K142" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:deploy": "date &amp;&amp; time npm-run-all ops:deploy:*",</v>
       </c>
       <c r="L142" s="2"/>
       <c r="M142" s="2"/>
       <c r="N142" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O142" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P142" t="str">
-        <f t="shared" ref="P142:P144" si="76">CONCATENATE(IF(CODE(I142)-CODE("a")&lt;0,LOWER(LEFT(I142,IF(ISERR(FIND(":",I142)),LEN(I142)+1,FIND(":",I142))-1)),I142),":*")</f>
+        <f t="shared" ref="P142:P144" si="77">CONCATENATE(IF(CODE(I142)-CODE("a")&lt;0,LOWER(LEFT(I142,IF(ISERR(FIND(":",I142)),LEN(I142)+1,FIND(":",I142))-1)),I142),":*")</f>
         <v>ops:deploy:*</v>
       </c>
     </row>
@@ -5504,23 +5516,23 @@
         <v>npm-run-all ops:deploy:package:*</v>
       </c>
       <c r="K143" t="str">
-        <f t="shared" si="36"/>
-        <v xml:space="preserve">    "ops:deploy:package": "echo date &amp;&amp; time npm-run-all ops:deploy:package:*",</v>
+        <f t="shared" si="73"/>
+        <v xml:space="preserve">    "ops:deploy:package": "date &amp;&amp; time echo npm-run-all ops:deploy:package:*",</v>
       </c>
       <c r="L143" s="2"/>
       <c r="M143" s="2">
         <v>1</v>
       </c>
       <c r="N143" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O143" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P143" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>ops:deploy:package:*</v>
       </c>
     </row>
@@ -5546,21 +5558,21 @@
         <v>npm-run-all ops:deploy:package:dockerize:*</v>
       </c>
       <c r="K144" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize": "date &amp;&amp; time npm-run-all ops:deploy:package:dockerize:*",</v>
       </c>
       <c r="L144" s="2"/>
       <c r="M144" s="2"/>
       <c r="N144" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O144" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P144" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>ops:deploy:package:dockerize:*</v>
       </c>
     </row>
@@ -5589,17 +5601,17 @@
         <v>npm-run-all ops:deploy:package:dockerize:build:action</v>
       </c>
       <c r="K145" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:build": "date &amp;&amp; time npm-run-all ops:deploy:package:dockerize:build:action",</v>
       </c>
       <c r="L145" s="2"/>
       <c r="M145" s="2"/>
       <c r="N145" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O145" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P145" t="str">
@@ -5632,17 +5644,17 @@
         <v>npm-run-all ops:deploy:package:dockerize:push:action</v>
       </c>
       <c r="K146" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:deploy:package:dockerize:push": "date &amp;&amp; time npm-run-all ops:deploy:package:dockerize:push:action",</v>
       </c>
       <c r="L146" s="2"/>
       <c r="M146" s="2"/>
       <c r="N146" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O146" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P146" t="str">
@@ -5672,17 +5684,17 @@
         <v>npm-run-all ops:deploy:package:provision:action</v>
       </c>
       <c r="K147" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:deploy:package:provision": "date &amp;&amp; time npm-run-all ops:deploy:package:provision:action",</v>
       </c>
       <c r="L147" s="2"/>
       <c r="M147" s="2"/>
       <c r="N147" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O147" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P147" t="str">
@@ -5712,17 +5724,17 @@
         <v>:</v>
       </c>
       <c r="K148" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:deploy:package:orchestrate": ":",</v>
       </c>
       <c r="L148" s="2"/>
       <c r="M148" s="2"/>
       <c r="N148" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O148" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5745,17 +5757,17 @@
         <v>:</v>
       </c>
       <c r="K149" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:deploy:report": ":",</v>
       </c>
       <c r="L149" s="2"/>
       <c r="M149" s="2"/>
       <c r="N149" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O149" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5784,21 +5796,21 @@
         <v>npm-run-all ops:run:*</v>
       </c>
       <c r="K150" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:run": "date &amp;&amp; time npm-run-all ops:run:*",</v>
       </c>
       <c r="L150" s="2"/>
       <c r="M150" s="2"/>
       <c r="N150" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O150" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P150" t="str">
-        <f t="shared" ref="P150" si="77">CONCATENATE(IF(CODE(I150)-CODE("a")&lt;0,LOWER(LEFT(I150,IF(ISERR(FIND(":",I150)),LEN(I150)+1,FIND(":",I150))-1)),I150),":*")</f>
+        <f t="shared" ref="P150" si="78">CONCATENATE(IF(CODE(I150)-CODE("a")&lt;0,LOWER(LEFT(I150,IF(ISERR(FIND(":",I150)),LEN(I150)+1,FIND(":",I150))-1)),I150),":*")</f>
         <v>ops:run:*</v>
       </c>
     </row>
@@ -5821,17 +5833,17 @@
         <v>npm-run-all ops:run:platform:action</v>
       </c>
       <c r="K151" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:run:platform": "date &amp;&amp; time npm-run-all ops:run:platform:action",</v>
       </c>
       <c r="L151" s="2"/>
       <c r="M151" s="2"/>
       <c r="N151" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O151" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P151" t="str">
@@ -5854,21 +5866,21 @@
         <v>ops:run:package</v>
       </c>
       <c r="J152" t="str">
-        <f t="shared" ref="J152:J168" si="78" xml:space="preserve"> IF(NOT(COUNTA(P152:V152)),":",_xlfn.TEXTJOIN(O152,TRUE,N152,_xlfn.TEXTJOIN(O152,TRUE,P152:V152)))</f>
+        <f t="shared" ref="J152:J168" si="79" xml:space="preserve"> IF(NOT(COUNTA(P152:V152)),":",_xlfn.TEXTJOIN(O152,TRUE,N152,_xlfn.TEXTJOIN(O152,TRUE,P152:V152)))</f>
         <v>:</v>
       </c>
       <c r="K152" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:run:package": ":",</v>
       </c>
       <c r="L152" s="2"/>
       <c r="M152" s="2"/>
       <c r="N152" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O152" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5887,21 +5899,21 @@
         <v>ops:run:chaos</v>
       </c>
       <c r="J153" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K153" t="str">
-        <f t="shared" ref="K153:K167" si="79">IF(ISBLANK(I153),"",CONCATENATE("    """,I153,""": ",IF(M153,"""echo ",""""),IF(LEN(J153)&gt;1,CONCATENATE(IF(L153,"",N$3)," "),""),J153,""","))</f>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:run:chaos": ":",</v>
       </c>
       <c r="L153" s="2"/>
       <c r="M153" s="2"/>
       <c r="N153" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O153" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5920,21 +5932,21 @@
         <v>ops:run:report</v>
       </c>
       <c r="J154" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K154" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:run:report": ":",</v>
       </c>
       <c r="L154" s="2"/>
       <c r="M154" s="2"/>
       <c r="N154" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O154" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5959,21 +5971,21 @@
         <v>ops:monitor</v>
       </c>
       <c r="J155" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>npm-run-all ops:monitor:*</v>
       </c>
       <c r="K155" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor": "date &amp;&amp; time npm-run-all ops:monitor:*",</v>
       </c>
       <c r="L155" s="2"/>
       <c r="M155" s="2"/>
       <c r="N155" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O155" s="2" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P155" t="str">
@@ -5996,17 +6008,17 @@
         <v>ops:monitor:platform</v>
       </c>
       <c r="J156" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K156" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:platform": ":",</v>
       </c>
       <c r="L156" s="2"/>
       <c r="M156" s="2"/>
       <c r="N156" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O156" s="2" t="str">
@@ -6029,17 +6041,17 @@
         <v>ops:monitor:package</v>
       </c>
       <c r="J157" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>npm-run-all ops:monitor:package:*</v>
       </c>
       <c r="K157" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:package": "date &amp;&amp; time npm-run-all ops:monitor:package:*",</v>
       </c>
       <c r="L157" s="2"/>
       <c r="M157" s="2"/>
       <c r="N157" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O157" s="2" t="str">
@@ -6069,17 +6081,17 @@
         <v>ops:monitor:package:trail</v>
       </c>
       <c r="J158" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>npm-run-all ops:monitor:package:trail:*</v>
       </c>
       <c r="K158" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:package:trail": "date &amp;&amp; time npm-run-all ops:monitor:package:trail:*",</v>
       </c>
       <c r="L158" s="2"/>
       <c r="M158" s="2"/>
       <c r="N158" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>npm-run-all</v>
       </c>
       <c r="O158" s="2" t="str">
@@ -6112,17 +6124,17 @@
         <v>ops:monitor:package:trail:health</v>
       </c>
       <c r="J159" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K159" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:health": ":",</v>
       </c>
       <c r="L159" s="2"/>
       <c r="M159" s="2"/>
       <c r="N159" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O159" s="2" t="str">
@@ -6151,17 +6163,17 @@
         <v>ops:monitor:package:trail:performance</v>
       </c>
       <c r="J160" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K160" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:performance": ":",</v>
       </c>
       <c r="L160" s="2"/>
       <c r="M160" s="2"/>
       <c r="N160" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O160" s="2" t="str">
@@ -6190,17 +6202,17 @@
         <v>ops:monitor:package:trail:resilience</v>
       </c>
       <c r="J161" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K161" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:resilience": ":",</v>
       </c>
       <c r="L161" s="2"/>
       <c r="M161" s="2"/>
       <c r="N161" s="2" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="O161" s="2" t="str">
@@ -6229,11 +6241,11 @@
         <v>ops:monitor:package:trail:security</v>
       </c>
       <c r="J162" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K162" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:package:trail:security": ":",</v>
       </c>
       <c r="L162" s="2"/>
@@ -6265,11 +6277,11 @@
         <v>ops:monitor:package:showcase</v>
       </c>
       <c r="J163" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K163" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:package:showcase": ":",</v>
       </c>
       <c r="L163" s="2"/>
@@ -6298,11 +6310,11 @@
         <v>ops:monitor:report</v>
       </c>
       <c r="J164" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>npm-run-all ops:monitor:report:action</v>
       </c>
       <c r="K164" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:monitor:report": "date &amp;&amp; time npm-run-all ops:monitor:report:action",</v>
       </c>
       <c r="L164" s="2"/>
@@ -6336,7 +6348,7 @@
         <v>:</v>
       </c>
       <c r="K165" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "ops:report": ":",</v>
       </c>
       <c r="L165" s="2"/>
@@ -6363,7 +6375,7 @@
         <v>:</v>
       </c>
       <c r="K166" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "report": ":",</v>
       </c>
       <c r="L166" s="2"/>
@@ -6379,10 +6391,10 @@
     </row>
     <row r="167" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E167" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I167" s="1" t="str">
         <f t="shared" si="91"/>
@@ -6393,7 +6405,7 @@
         <v>npm-run-all pipeline:finish:action</v>
       </c>
       <c r="K167" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="73"/>
         <v xml:space="preserve">    "pipeline:finish": "date &amp;&amp; time npm-run-all pipeline:finish:action",</v>
       </c>
       <c r="L167" s="2"/>
@@ -6420,11 +6432,11 @@
         <v>// END PIPELINE</v>
       </c>
       <c r="J168" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>:</v>
       </c>
       <c r="K168" t="str">
-        <f>IF(ISBLANK(I168),"",CONCATENATE("    """,I168,""": ",IF(M168,"""echo ",""""),IF(LEN(J168)&gt;1,CONCATENATE(IF(L168,"",N$3)," "),""),J168,""""))</f>
+        <f>IF(ISBLANK(I168),"",CONCATENATE("    """,I168,""": ","""",IF(LEN(J168)&gt;1,CONCATENATE(IF(L168,"",CONCATENATE(N$3," ")),""),""),IF(M168,"echo ",""),J168,""""))</f>
         <v xml:space="preserve">    "// END PIPELINE": ":"</v>
       </c>
       <c r="L168" s="2"/>
@@ -6481,7 +6493,7 @@
       </c>
       <c r="L170">
         <f>COUNTA(L8:L168)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M170">
         <f>COUNTA(M8:M168)</f>

</xml_diff>